<commit_message>
[dev] startlocation Random 위치 추가
1. startlocation Random 위치 추가
1.1 target_near 구현
1.2 target_random 구현
1.3 TargetLocation 중 target_random과 target_direction 구분 필요
</commit_message>
<xml_diff>
--- a/Assets/300_Data/ExcelData/SkillDataTable.xlsx
+++ b/Assets/300_Data/ExcelData/SkillDataTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Unity\Project\LevelDesignDev\LevelDesignDev\Assets\300_Data\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B19A8C45-4921-412C-B34B-1323389A4382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F74712DF-8A82-44B2-B3A8-C645E4738E82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="645" yWindow="1395" windowWidth="17445" windowHeight="14355" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1155" yWindow="1215" windowWidth="17445" windowHeight="14355" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SkillRule" sheetId="3" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="927" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="422">
   <si>
     <t># skill_information</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -1574,6 +1574,17 @@
   </si>
   <si>
     <t>S_Fireball</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>PrefabID</t>
+  </si>
+  <si>
+    <t>프리팹 키</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>가져올 프리팹의 ID</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -2007,34 +2018,13 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2049,23 +2039,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2083,6 +2064,18 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2090,24 +2083,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2124,9 +2099,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2136,8 +2108,47 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2419,10 +2430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CA75FAF-DEF9-4E16-8BC9-F0A67872783F}">
-  <dimension ref="B3:S91"/>
+  <dimension ref="B3:S92"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8:O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2450,1837 +2461,1837 @@
       <c r="O3" s="3"/>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B4" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26" t="s">
+      <c r="B4" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="27"/>
-      <c r="F4" s="28" t="s">
+      <c r="E4" s="57"/>
+      <c r="F4" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26" t="s">
+      <c r="G4" s="56"/>
+      <c r="H4" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="26"/>
-      <c r="M4" s="26"/>
-      <c r="N4" s="26"/>
-      <c r="O4" s="26"/>
-      <c r="P4" s="26" t="s">
+      <c r="I4" s="56"/>
+      <c r="J4" s="56"/>
+      <c r="K4" s="56"/>
+      <c r="L4" s="56"/>
+      <c r="M4" s="56"/>
+      <c r="N4" s="56"/>
+      <c r="O4" s="56"/>
+      <c r="P4" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="Q4" s="26"/>
-      <c r="R4" s="26"/>
-      <c r="S4" s="26"/>
+      <c r="Q4" s="56"/>
+      <c r="R4" s="56"/>
+      <c r="S4" s="56"/>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="30"/>
-      <c r="D5" s="29" t="s">
+      <c r="C5" s="64"/>
+      <c r="D5" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="31"/>
+      <c r="E5" s="65"/>
       <c r="F5" s="5" t="s">
         <v>8</v>
       </c>
       <c r="G5" s="6"/>
-      <c r="H5" s="32" t="s">
+      <c r="H5" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="32"/>
-      <c r="L5" s="32"/>
-      <c r="M5" s="32"/>
-      <c r="N5" s="32"/>
-      <c r="O5" s="32"/>
-      <c r="P5" s="32"/>
-      <c r="Q5" s="32"/>
-      <c r="R5" s="32"/>
-      <c r="S5" s="32"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="28"/>
+      <c r="N5" s="28"/>
+      <c r="O5" s="28"/>
+      <c r="P5" s="28"/>
+      <c r="Q5" s="28"/>
+      <c r="R5" s="28"/>
+      <c r="S5" s="28"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="30"/>
-      <c r="D6" s="29" t="s">
+      <c r="C6" s="64"/>
+      <c r="D6" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="31"/>
+      <c r="E6" s="65"/>
       <c r="F6" s="5" t="s">
         <v>12</v>
       </c>
       <c r="G6" s="6"/>
-      <c r="H6" s="33" t="s">
+      <c r="H6" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="34"/>
-      <c r="J6" s="34"/>
-      <c r="K6" s="34"/>
-      <c r="L6" s="34"/>
-      <c r="M6" s="34"/>
-      <c r="N6" s="34"/>
-      <c r="O6" s="35"/>
-      <c r="P6" s="32"/>
-      <c r="Q6" s="32"/>
-      <c r="R6" s="32"/>
-      <c r="S6" s="32"/>
+      <c r="I6" s="67"/>
+      <c r="J6" s="67"/>
+      <c r="K6" s="67"/>
+      <c r="L6" s="67"/>
+      <c r="M6" s="67"/>
+      <c r="N6" s="67"/>
+      <c r="O6" s="68"/>
+      <c r="P6" s="28"/>
+      <c r="Q6" s="28"/>
+      <c r="R6" s="28"/>
+      <c r="S6" s="28"/>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="30"/>
-      <c r="D7" s="29" t="s">
+      <c r="C7" s="64"/>
+      <c r="D7" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="31"/>
+      <c r="E7" s="65"/>
       <c r="F7" s="5" t="s">
         <v>16</v>
       </c>
       <c r="G7" s="6"/>
-      <c r="H7" s="33" t="s">
+      <c r="H7" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="34"/>
-      <c r="J7" s="34"/>
-      <c r="K7" s="34"/>
-      <c r="L7" s="34"/>
-      <c r="M7" s="34"/>
-      <c r="N7" s="34"/>
-      <c r="O7" s="35"/>
-      <c r="P7" s="32"/>
-      <c r="Q7" s="32"/>
-      <c r="R7" s="32"/>
-      <c r="S7" s="32"/>
+      <c r="I7" s="67"/>
+      <c r="J7" s="67"/>
+      <c r="K7" s="67"/>
+      <c r="L7" s="67"/>
+      <c r="M7" s="67"/>
+      <c r="N7" s="67"/>
+      <c r="O7" s="68"/>
+      <c r="P7" s="66"/>
+      <c r="Q7" s="67"/>
+      <c r="R7" s="67"/>
+      <c r="S7" s="68"/>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="27" t="s">
+        <v>419</v>
+      </c>
+      <c r="C8" s="64"/>
+      <c r="D8" s="27" t="s">
+        <v>420</v>
+      </c>
+      <c r="E8" s="65"/>
+      <c r="F8" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="G8" s="6"/>
+      <c r="H8" s="66" t="s">
+        <v>421</v>
+      </c>
+      <c r="I8" s="67"/>
+      <c r="J8" s="67"/>
+      <c r="K8" s="67"/>
+      <c r="L8" s="67"/>
+      <c r="M8" s="67"/>
+      <c r="N8" s="67"/>
+      <c r="O8" s="68"/>
+      <c r="P8" s="28"/>
+      <c r="Q8" s="28"/>
+      <c r="R8" s="28"/>
+      <c r="S8" s="28"/>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B9" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="30"/>
-      <c r="D8" s="29" t="s">
+      <c r="C9" s="64"/>
+      <c r="D9" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="31"/>
-      <c r="F8" s="5" t="s">
+      <c r="E9" s="65"/>
+      <c r="F9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="6"/>
-      <c r="H8" s="33" t="s">
+      <c r="G9" s="6"/>
+      <c r="H9" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="34"/>
-      <c r="J8" s="34"/>
-      <c r="K8" s="34"/>
-      <c r="L8" s="34"/>
-      <c r="M8" s="34"/>
-      <c r="N8" s="34"/>
-      <c r="O8" s="35"/>
-      <c r="P8" s="32"/>
-      <c r="Q8" s="32"/>
-      <c r="R8" s="32"/>
-      <c r="S8" s="32"/>
-    </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B9" s="29" t="s">
+      <c r="I9" s="67"/>
+      <c r="J9" s="67"/>
+      <c r="K9" s="67"/>
+      <c r="L9" s="67"/>
+      <c r="M9" s="67"/>
+      <c r="N9" s="67"/>
+      <c r="O9" s="68"/>
+      <c r="P9" s="28"/>
+      <c r="Q9" s="28"/>
+      <c r="R9" s="28"/>
+      <c r="S9" s="28"/>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B10" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="30"/>
-      <c r="D9" s="29" t="s">
+      <c r="C10" s="64"/>
+      <c r="D10" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="31"/>
-      <c r="F9" s="5" t="s">
+      <c r="E10" s="65"/>
+      <c r="F10" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G9" s="6"/>
-      <c r="H9" s="33" t="s">
+      <c r="G10" s="6"/>
+      <c r="H10" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="I9" s="34"/>
-      <c r="J9" s="34"/>
-      <c r="K9" s="34"/>
-      <c r="L9" s="34"/>
-      <c r="M9" s="34"/>
-      <c r="N9" s="34"/>
-      <c r="O9" s="35"/>
-      <c r="P9" s="32"/>
-      <c r="Q9" s="32"/>
-      <c r="R9" s="32"/>
-      <c r="S9" s="32"/>
-    </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B10" s="29" t="s">
+      <c r="I10" s="67"/>
+      <c r="J10" s="67"/>
+      <c r="K10" s="67"/>
+      <c r="L10" s="67"/>
+      <c r="M10" s="67"/>
+      <c r="N10" s="67"/>
+      <c r="O10" s="68"/>
+      <c r="P10" s="28"/>
+      <c r="Q10" s="28"/>
+      <c r="R10" s="28"/>
+      <c r="S10" s="28"/>
+    </row>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B11" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="30"/>
-      <c r="D10" s="29" t="s">
+      <c r="C11" s="64"/>
+      <c r="D11" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="31"/>
-      <c r="F10" s="5" t="s">
+      <c r="E11" s="65"/>
+      <c r="F11" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="33" t="s">
+      <c r="G11" s="6"/>
+      <c r="H11" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="I10" s="34"/>
-      <c r="J10" s="34"/>
-      <c r="K10" s="34"/>
-      <c r="L10" s="34"/>
-      <c r="M10" s="34"/>
-      <c r="N10" s="34"/>
-      <c r="O10" s="35"/>
-      <c r="P10" s="32"/>
-      <c r="Q10" s="32"/>
-      <c r="R10" s="32"/>
-      <c r="S10" s="32"/>
-    </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B11" s="29" t="s">
+      <c r="I11" s="67"/>
+      <c r="J11" s="67"/>
+      <c r="K11" s="67"/>
+      <c r="L11" s="67"/>
+      <c r="M11" s="67"/>
+      <c r="N11" s="67"/>
+      <c r="O11" s="68"/>
+      <c r="P11" s="28"/>
+      <c r="Q11" s="28"/>
+      <c r="R11" s="28"/>
+      <c r="S11" s="28"/>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B12" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="30"/>
-      <c r="D11" s="29" t="s">
+      <c r="C12" s="64"/>
+      <c r="D12" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="31"/>
-      <c r="F11" s="5" t="s">
+      <c r="E12" s="65"/>
+      <c r="F12" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="6"/>
-      <c r="H11" s="33" t="s">
+      <c r="G12" s="6"/>
+      <c r="H12" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="I11" s="34"/>
-      <c r="J11" s="34"/>
-      <c r="K11" s="34"/>
-      <c r="L11" s="34"/>
-      <c r="M11" s="34"/>
-      <c r="N11" s="34"/>
-      <c r="O11" s="35"/>
-      <c r="P11" s="32" t="s">
+      <c r="I12" s="67"/>
+      <c r="J12" s="67"/>
+      <c r="K12" s="67"/>
+      <c r="L12" s="67"/>
+      <c r="M12" s="67"/>
+      <c r="N12" s="67"/>
+      <c r="O12" s="68"/>
+      <c r="P12" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="Q11" s="32"/>
-      <c r="R11" s="32"/>
-      <c r="S11" s="32"/>
-    </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B12" s="29" t="s">
+      <c r="Q12" s="28"/>
+      <c r="R12" s="28"/>
+      <c r="S12" s="28"/>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B13" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="30"/>
-      <c r="D12" s="29" t="s">
+      <c r="C13" s="64"/>
+      <c r="D13" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="31"/>
-      <c r="F12" s="5" t="s">
+      <c r="E13" s="65"/>
+      <c r="F13" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G12" s="6"/>
-      <c r="H12" s="33" t="s">
+      <c r="G13" s="6"/>
+      <c r="H13" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="I12" s="34"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="34"/>
-      <c r="L12" s="34"/>
-      <c r="M12" s="34"/>
-      <c r="N12" s="34"/>
-      <c r="O12" s="35"/>
-      <c r="P12" s="32"/>
-      <c r="Q12" s="32"/>
-      <c r="R12" s="32"/>
-      <c r="S12" s="32"/>
-    </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B13" s="29" t="s">
+      <c r="I13" s="67"/>
+      <c r="J13" s="67"/>
+      <c r="K13" s="67"/>
+      <c r="L13" s="67"/>
+      <c r="M13" s="67"/>
+      <c r="N13" s="67"/>
+      <c r="O13" s="68"/>
+      <c r="P13" s="28"/>
+      <c r="Q13" s="28"/>
+      <c r="R13" s="28"/>
+      <c r="S13" s="28"/>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B14" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="30"/>
-      <c r="D13" s="29" t="s">
+      <c r="C14" s="64"/>
+      <c r="D14" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="E13" s="31"/>
-      <c r="F13" s="5" t="s">
+      <c r="E14" s="65"/>
+      <c r="F14" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G13" s="6"/>
-      <c r="H13" s="33" t="s">
+      <c r="G14" s="6"/>
+      <c r="H14" s="66" t="s">
         <v>40</v>
       </c>
-      <c r="I13" s="34"/>
-      <c r="J13" s="34"/>
-      <c r="K13" s="34"/>
-      <c r="L13" s="34"/>
-      <c r="M13" s="34"/>
-      <c r="N13" s="34"/>
-      <c r="O13" s="35"/>
-      <c r="P13" s="32" t="s">
+      <c r="I14" s="67"/>
+      <c r="J14" s="67"/>
+      <c r="K14" s="67"/>
+      <c r="L14" s="67"/>
+      <c r="M14" s="67"/>
+      <c r="N14" s="67"/>
+      <c r="O14" s="68"/>
+      <c r="P14" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="Q13" s="32"/>
-      <c r="R13" s="32"/>
-      <c r="S13" s="32"/>
-    </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B14" s="29" t="s">
+      <c r="Q14" s="28"/>
+      <c r="R14" s="28"/>
+      <c r="S14" s="28"/>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B15" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="30"/>
-      <c r="D14" s="29" t="s">
+      <c r="C15" s="64"/>
+      <c r="D15" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="E14" s="31"/>
-      <c r="F14" s="5" t="s">
+      <c r="E15" s="65"/>
+      <c r="F15" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="G14" s="6"/>
-      <c r="H14" s="33" t="s">
+      <c r="G15" s="6"/>
+      <c r="H15" s="66" t="s">
         <v>44</v>
       </c>
-      <c r="I14" s="34"/>
-      <c r="J14" s="34"/>
-      <c r="K14" s="34"/>
-      <c r="L14" s="34"/>
-      <c r="M14" s="34"/>
-      <c r="N14" s="34"/>
-      <c r="O14" s="35"/>
-      <c r="P14" s="32"/>
-      <c r="Q14" s="32"/>
-      <c r="R14" s="32"/>
-      <c r="S14" s="32"/>
-    </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B15" s="36" t="s">
+      <c r="I15" s="67"/>
+      <c r="J15" s="67"/>
+      <c r="K15" s="67"/>
+      <c r="L15" s="67"/>
+      <c r="M15" s="67"/>
+      <c r="N15" s="67"/>
+      <c r="O15" s="68"/>
+      <c r="P15" s="28"/>
+      <c r="Q15" s="28"/>
+      <c r="R15" s="28"/>
+      <c r="S15" s="28"/>
+    </row>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B16" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="37"/>
-      <c r="D15" s="36" t="s">
+      <c r="C16" s="30"/>
+      <c r="D16" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="42"/>
-      <c r="F15" s="5" t="s">
+      <c r="E16" s="33"/>
+      <c r="F16" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="G15" s="6"/>
-      <c r="H15" s="33" t="s">
+      <c r="G16" s="6"/>
+      <c r="H16" s="66" t="s">
         <v>48</v>
       </c>
-      <c r="I15" s="34"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="34"/>
-      <c r="L15" s="34"/>
-      <c r="M15" s="34"/>
-      <c r="N15" s="34"/>
-      <c r="O15" s="35"/>
-      <c r="P15" s="45" t="s">
+      <c r="I16" s="67"/>
+      <c r="J16" s="67"/>
+      <c r="K16" s="67"/>
+      <c r="L16" s="67"/>
+      <c r="M16" s="67"/>
+      <c r="N16" s="67"/>
+      <c r="O16" s="68"/>
+      <c r="P16" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="Q15" s="46"/>
-      <c r="R15" s="46"/>
-      <c r="S15" s="47"/>
-    </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B16" s="38"/>
-      <c r="C16" s="39"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="43"/>
-      <c r="F16" s="5" t="s">
+      <c r="Q16" s="36"/>
+      <c r="R16" s="36"/>
+      <c r="S16" s="37"/>
+    </row>
+    <row r="17" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B17" s="31"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="G16" s="6"/>
-      <c r="H16" s="33" t="s">
+      <c r="G17" s="6"/>
+      <c r="H17" s="66" t="s">
         <v>51</v>
       </c>
-      <c r="I16" s="34"/>
-      <c r="J16" s="34"/>
-      <c r="K16" s="34"/>
-      <c r="L16" s="34"/>
-      <c r="M16" s="34"/>
-      <c r="N16" s="34"/>
-      <c r="O16" s="35"/>
-      <c r="P16" s="48"/>
-      <c r="Q16" s="49"/>
-      <c r="R16" s="49"/>
-      <c r="S16" s="50"/>
-    </row>
-    <row r="17" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B17" s="40"/>
-      <c r="C17" s="41"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="44"/>
-      <c r="F17" s="5" t="s">
+      <c r="I17" s="67"/>
+      <c r="J17" s="67"/>
+      <c r="K17" s="67"/>
+      <c r="L17" s="67"/>
+      <c r="M17" s="67"/>
+      <c r="N17" s="67"/>
+      <c r="O17" s="68"/>
+      <c r="P17" s="38"/>
+      <c r="Q17" s="39"/>
+      <c r="R17" s="39"/>
+      <c r="S17" s="40"/>
+    </row>
+    <row r="18" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B18" s="41"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="G17" s="6"/>
-      <c r="H17" s="33" t="s">
+      <c r="G18" s="6"/>
+      <c r="H18" s="66" t="s">
         <v>53</v>
       </c>
-      <c r="I17" s="34"/>
-      <c r="J17" s="34"/>
-      <c r="K17" s="34"/>
-      <c r="L17" s="34"/>
-      <c r="M17" s="34"/>
-      <c r="N17" s="34"/>
-      <c r="O17" s="35"/>
-      <c r="P17" s="51"/>
-      <c r="Q17" s="52"/>
-      <c r="R17" s="52"/>
-      <c r="S17" s="53"/>
-    </row>
-    <row r="21" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B21" s="2" t="s">
+      <c r="I18" s="67"/>
+      <c r="J18" s="67"/>
+      <c r="K18" s="67"/>
+      <c r="L18" s="67"/>
+      <c r="M18" s="67"/>
+      <c r="N18" s="67"/>
+      <c r="O18" s="68"/>
+      <c r="P18" s="45"/>
+      <c r="Q18" s="46"/>
+      <c r="R18" s="46"/>
+      <c r="S18" s="47"/>
+    </row>
+    <row r="22" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B22" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-      <c r="O21" s="3"/>
-    </row>
-    <row r="22" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B22" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="C22" s="26"/>
-      <c r="D22" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="E22" s="27"/>
-      <c r="F22" s="54" t="s">
-        <v>3</v>
-      </c>
-      <c r="G22" s="55"/>
-      <c r="H22" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="I22" s="26"/>
-      <c r="J22" s="26"/>
-      <c r="K22" s="26"/>
-      <c r="L22" s="26"/>
-      <c r="M22" s="26"/>
-      <c r="N22" s="26"/>
-      <c r="O22" s="26"/>
-      <c r="P22" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q22" s="26"/>
-      <c r="R22" s="26"/>
-      <c r="S22" s="26"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B23" s="56" t="s">
-        <v>55</v>
+        <v>1</v>
       </c>
       <c r="C23" s="56"/>
       <c r="D23" s="56" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23" s="57"/>
+      <c r="F23" s="58" t="s">
+        <v>3</v>
+      </c>
+      <c r="G23" s="59"/>
+      <c r="H23" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="I23" s="56"/>
+      <c r="J23" s="56"/>
+      <c r="K23" s="56"/>
+      <c r="L23" s="56"/>
+      <c r="M23" s="56"/>
+      <c r="N23" s="56"/>
+      <c r="O23" s="56"/>
+      <c r="P23" s="56" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q23" s="56"/>
+      <c r="R23" s="56"/>
+      <c r="S23" s="56"/>
+    </row>
+    <row r="24" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B24" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="E23" s="29"/>
-      <c r="F23" s="5" t="s">
+      <c r="E24" s="27"/>
+      <c r="F24" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="G23" s="6"/>
-      <c r="H23" s="32" t="s">
+      <c r="G24" s="6"/>
+      <c r="H24" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="I23" s="32"/>
-      <c r="J23" s="32"/>
-      <c r="K23" s="32"/>
-      <c r="L23" s="32"/>
-      <c r="M23" s="32"/>
-      <c r="N23" s="32"/>
-      <c r="O23" s="32"/>
-      <c r="P23" s="32" t="s">
+      <c r="I24" s="28"/>
+      <c r="J24" s="28"/>
+      <c r="K24" s="28"/>
+      <c r="L24" s="28"/>
+      <c r="M24" s="28"/>
+      <c r="N24" s="28"/>
+      <c r="O24" s="28"/>
+      <c r="P24" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="Q23" s="32"/>
-      <c r="R23" s="32"/>
-      <c r="S23" s="32"/>
-    </row>
-    <row r="24" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="36" t="s">
+      <c r="Q24" s="28"/>
+      <c r="R24" s="28"/>
+      <c r="S24" s="28"/>
+    </row>
+    <row r="25" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="C24" s="37"/>
-      <c r="D24" s="36" t="s">
+      <c r="C25" s="30"/>
+      <c r="D25" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="E24" s="57"/>
-      <c r="F24" s="7" t="s">
+      <c r="E25" s="61"/>
+      <c r="F25" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="G24" s="8"/>
-      <c r="H24" s="59" t="s">
+      <c r="G25" s="8"/>
+      <c r="H25" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="I24" s="60"/>
-      <c r="J24" s="60"/>
-      <c r="K24" s="60"/>
-      <c r="L24" s="60"/>
-      <c r="M24" s="60"/>
-      <c r="N24" s="60"/>
-      <c r="O24" s="61"/>
-      <c r="P24" s="45" t="s">
+      <c r="I25" s="48"/>
+      <c r="J25" s="48"/>
+      <c r="K25" s="48"/>
+      <c r="L25" s="48"/>
+      <c r="M25" s="48"/>
+      <c r="N25" s="48"/>
+      <c r="O25" s="49"/>
+      <c r="P25" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="Q24" s="46"/>
-      <c r="R24" s="46"/>
-      <c r="S24" s="47"/>
-    </row>
-    <row r="25" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="40"/>
-      <c r="C25" s="41"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="58"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="62"/>
-      <c r="I25" s="63"/>
-      <c r="J25" s="63"/>
-      <c r="K25" s="63"/>
-      <c r="L25" s="63"/>
-      <c r="M25" s="63"/>
-      <c r="N25" s="63"/>
-      <c r="O25" s="64"/>
-      <c r="P25" s="51"/>
-      <c r="Q25" s="52"/>
-      <c r="R25" s="52"/>
-      <c r="S25" s="53"/>
-    </row>
-    <row r="26" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B26" s="36" t="s">
-        <v>65</v>
-      </c>
-      <c r="C26" s="37"/>
-      <c r="D26" s="36" t="s">
-        <v>66</v>
-      </c>
-      <c r="E26" s="57"/>
-      <c r="F26" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="G26" s="6"/>
-      <c r="H26" s="65" t="s">
-        <v>67</v>
-      </c>
-      <c r="I26" s="65"/>
-      <c r="J26" s="65"/>
-      <c r="K26" s="65"/>
-      <c r="L26" s="65"/>
-      <c r="M26" s="65"/>
-      <c r="N26" s="65"/>
-      <c r="O26" s="65"/>
-      <c r="P26" s="45" t="s">
-        <v>68</v>
-      </c>
+      <c r="Q25" s="36"/>
+      <c r="R25" s="36"/>
+      <c r="S25" s="37"/>
+    </row>
+    <row r="26" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="41"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="41"/>
+      <c r="E26" s="62"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="50"/>
+      <c r="I26" s="51"/>
+      <c r="J26" s="51"/>
+      <c r="K26" s="51"/>
+      <c r="L26" s="51"/>
+      <c r="M26" s="51"/>
+      <c r="N26" s="51"/>
+      <c r="O26" s="52"/>
+      <c r="P26" s="45"/>
       <c r="Q26" s="46"/>
       <c r="R26" s="46"/>
       <c r="S26" s="47"/>
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B27" s="40"/>
-      <c r="C27" s="41"/>
-      <c r="D27" s="40"/>
-      <c r="E27" s="58"/>
+      <c r="B27" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" s="30"/>
+      <c r="D27" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="E27" s="61"/>
       <c r="F27" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G27" s="6"/>
-      <c r="H27" s="65" t="s">
+      <c r="H27" s="63" t="s">
+        <v>67</v>
+      </c>
+      <c r="I27" s="63"/>
+      <c r="J27" s="63"/>
+      <c r="K27" s="63"/>
+      <c r="L27" s="63"/>
+      <c r="M27" s="63"/>
+      <c r="N27" s="63"/>
+      <c r="O27" s="63"/>
+      <c r="P27" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q27" s="36"/>
+      <c r="R27" s="36"/>
+      <c r="S27" s="37"/>
+    </row>
+    <row r="28" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B28" s="41"/>
+      <c r="C28" s="42"/>
+      <c r="D28" s="41"/>
+      <c r="E28" s="62"/>
+      <c r="F28" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="G28" s="6"/>
+      <c r="H28" s="63" t="s">
         <v>69</v>
       </c>
-      <c r="I27" s="65"/>
-      <c r="J27" s="65"/>
-      <c r="K27" s="65"/>
-      <c r="L27" s="65"/>
-      <c r="M27" s="65"/>
-      <c r="N27" s="65"/>
-      <c r="O27" s="65"/>
-      <c r="P27" s="51"/>
-      <c r="Q27" s="52"/>
-      <c r="R27" s="52"/>
-      <c r="S27" s="53"/>
-    </row>
-    <row r="31" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B31" s="2" t="s">
+      <c r="I28" s="63"/>
+      <c r="J28" s="63"/>
+      <c r="K28" s="63"/>
+      <c r="L28" s="63"/>
+      <c r="M28" s="63"/>
+      <c r="N28" s="63"/>
+      <c r="O28" s="63"/>
+      <c r="P28" s="45"/>
+      <c r="Q28" s="46"/>
+      <c r="R28" s="46"/>
+      <c r="S28" s="47"/>
+    </row>
+    <row r="32" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B32" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B32" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="C32" s="26"/>
-      <c r="D32" s="26" t="s">
+    <row r="33" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B33" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" s="56"/>
+      <c r="D33" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="E32" s="27"/>
-      <c r="F32" s="54" t="s">
+      <c r="E33" s="57"/>
+      <c r="F33" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="G32" s="55"/>
-      <c r="H32" s="26" t="s">
+      <c r="G33" s="59"/>
+      <c r="H33" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="I32" s="26"/>
-      <c r="J32" s="26"/>
-      <c r="K32" s="26"/>
-      <c r="L32" s="26"/>
-      <c r="M32" s="26"/>
-      <c r="N32" s="26"/>
-      <c r="O32" s="26"/>
-      <c r="P32" s="26" t="s">
+      <c r="I33" s="56"/>
+      <c r="J33" s="56"/>
+      <c r="K33" s="56"/>
+      <c r="L33" s="56"/>
+      <c r="M33" s="56"/>
+      <c r="N33" s="56"/>
+      <c r="O33" s="56"/>
+      <c r="P33" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="Q32" s="26"/>
-      <c r="R32" s="26"/>
-      <c r="S32" s="26"/>
-    </row>
-    <row r="33" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B33" s="36" t="s">
+      <c r="Q33" s="56"/>
+      <c r="R33" s="56"/>
+      <c r="S33" s="56"/>
+    </row>
+    <row r="34" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B34" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="C33" s="37"/>
-      <c r="D33" s="36" t="s">
+      <c r="C34" s="30"/>
+      <c r="D34" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="E33" s="42"/>
-      <c r="F33" s="5" t="s">
+      <c r="E34" s="33"/>
+      <c r="F34" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="G33" s="6"/>
-      <c r="H33" s="32" t="s">
+      <c r="G34" s="6"/>
+      <c r="H34" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="I33" s="32"/>
-      <c r="J33" s="32"/>
-      <c r="K33" s="32"/>
-      <c r="L33" s="32"/>
-      <c r="M33" s="32"/>
-      <c r="N33" s="32"/>
-      <c r="O33" s="32"/>
-      <c r="P33" s="59" t="s">
+      <c r="I34" s="28"/>
+      <c r="J34" s="28"/>
+      <c r="K34" s="28"/>
+      <c r="L34" s="28"/>
+      <c r="M34" s="28"/>
+      <c r="N34" s="28"/>
+      <c r="O34" s="28"/>
+      <c r="P34" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="Q33" s="46"/>
-      <c r="R33" s="46"/>
-      <c r="S33" s="47"/>
-    </row>
-    <row r="34" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B34" s="38"/>
-      <c r="C34" s="39"/>
-      <c r="D34" s="38"/>
-      <c r="E34" s="43"/>
-      <c r="F34" s="5" t="s">
+      <c r="Q34" s="36"/>
+      <c r="R34" s="36"/>
+      <c r="S34" s="37"/>
+    </row>
+    <row r="35" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B35" s="31"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="G34" s="6"/>
-      <c r="H34" s="32" t="s">
+      <c r="G35" s="6"/>
+      <c r="H35" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="I34" s="32"/>
-      <c r="J34" s="32"/>
-      <c r="K34" s="32"/>
-      <c r="L34" s="32"/>
-      <c r="M34" s="32"/>
-      <c r="N34" s="32"/>
-      <c r="O34" s="32"/>
-      <c r="P34" s="48"/>
-      <c r="Q34" s="49"/>
-      <c r="R34" s="49"/>
-      <c r="S34" s="50"/>
-    </row>
-    <row r="35" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B35" s="38"/>
-      <c r="C35" s="39"/>
-      <c r="D35" s="38"/>
-      <c r="E35" s="43"/>
-      <c r="F35" s="5" t="s">
+      <c r="I35" s="28"/>
+      <c r="J35" s="28"/>
+      <c r="K35" s="28"/>
+      <c r="L35" s="28"/>
+      <c r="M35" s="28"/>
+      <c r="N35" s="28"/>
+      <c r="O35" s="28"/>
+      <c r="P35" s="38"/>
+      <c r="Q35" s="39"/>
+      <c r="R35" s="39"/>
+      <c r="S35" s="40"/>
+    </row>
+    <row r="36" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B36" s="31"/>
+      <c r="C36" s="32"/>
+      <c r="D36" s="31"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="G35" s="6"/>
-      <c r="H35" s="32" t="s">
+      <c r="G36" s="6"/>
+      <c r="H36" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="I35" s="32"/>
-      <c r="J35" s="32"/>
-      <c r="K35" s="32"/>
-      <c r="L35" s="32"/>
-      <c r="M35" s="32"/>
-      <c r="N35" s="32"/>
-      <c r="O35" s="32"/>
-      <c r="P35" s="48"/>
-      <c r="Q35" s="49"/>
-      <c r="R35" s="49"/>
-      <c r="S35" s="50"/>
-    </row>
-    <row r="36" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B36" s="38"/>
-      <c r="C36" s="39"/>
-      <c r="D36" s="38"/>
-      <c r="E36" s="43"/>
-      <c r="F36" s="5" t="s">
+      <c r="I36" s="28"/>
+      <c r="J36" s="28"/>
+      <c r="K36" s="28"/>
+      <c r="L36" s="28"/>
+      <c r="M36" s="28"/>
+      <c r="N36" s="28"/>
+      <c r="O36" s="28"/>
+      <c r="P36" s="38"/>
+      <c r="Q36" s="39"/>
+      <c r="R36" s="39"/>
+      <c r="S36" s="40"/>
+    </row>
+    <row r="37" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B37" s="31"/>
+      <c r="C37" s="32"/>
+      <c r="D37" s="31"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="G36" s="6"/>
-      <c r="H36" s="32" t="s">
+      <c r="G37" s="6"/>
+      <c r="H37" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="I36" s="32"/>
-      <c r="J36" s="32"/>
-      <c r="K36" s="32"/>
-      <c r="L36" s="32"/>
-      <c r="M36" s="32"/>
-      <c r="N36" s="32"/>
-      <c r="O36" s="32"/>
-      <c r="P36" s="48"/>
-      <c r="Q36" s="49"/>
-      <c r="R36" s="49"/>
-      <c r="S36" s="50"/>
-    </row>
-    <row r="37" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B37" s="40"/>
-      <c r="C37" s="41"/>
-      <c r="D37" s="40"/>
-      <c r="E37" s="44"/>
-      <c r="F37" s="5" t="s">
+      <c r="I37" s="28"/>
+      <c r="J37" s="28"/>
+      <c r="K37" s="28"/>
+      <c r="L37" s="28"/>
+      <c r="M37" s="28"/>
+      <c r="N37" s="28"/>
+      <c r="O37" s="28"/>
+      <c r="P37" s="38"/>
+      <c r="Q37" s="39"/>
+      <c r="R37" s="39"/>
+      <c r="S37" s="40"/>
+    </row>
+    <row r="38" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B38" s="41"/>
+      <c r="C38" s="42"/>
+      <c r="D38" s="41"/>
+      <c r="E38" s="43"/>
+      <c r="F38" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="G37" s="6"/>
-      <c r="H37" s="32" t="s">
+      <c r="G38" s="6"/>
+      <c r="H38" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="I37" s="32"/>
-      <c r="J37" s="32"/>
-      <c r="K37" s="32"/>
-      <c r="L37" s="32"/>
-      <c r="M37" s="32"/>
-      <c r="N37" s="32"/>
-      <c r="O37" s="32"/>
-      <c r="P37" s="51"/>
-      <c r="Q37" s="52"/>
-      <c r="R37" s="52"/>
-      <c r="S37" s="53"/>
-    </row>
-    <row r="38" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B38" s="36" t="s">
+      <c r="I38" s="28"/>
+      <c r="J38" s="28"/>
+      <c r="K38" s="28"/>
+      <c r="L38" s="28"/>
+      <c r="M38" s="28"/>
+      <c r="N38" s="28"/>
+      <c r="O38" s="28"/>
+      <c r="P38" s="45"/>
+      <c r="Q38" s="46"/>
+      <c r="R38" s="46"/>
+      <c r="S38" s="47"/>
+    </row>
+    <row r="39" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B39" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="C38" s="37"/>
-      <c r="D38" s="36" t="s">
+      <c r="C39" s="30"/>
+      <c r="D39" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="E38" s="42"/>
-      <c r="F38" s="5" t="s">
+      <c r="E39" s="33"/>
+      <c r="F39" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="G38" s="6"/>
-      <c r="H38" s="32" t="s">
+      <c r="G39" s="6"/>
+      <c r="H39" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="I38" s="32"/>
-      <c r="J38" s="32"/>
-      <c r="K38" s="32"/>
-      <c r="L38" s="32"/>
-      <c r="M38" s="32"/>
-      <c r="N38" s="32"/>
-      <c r="O38" s="32"/>
-      <c r="P38" s="59" t="s">
+      <c r="I39" s="28"/>
+      <c r="J39" s="28"/>
+      <c r="K39" s="28"/>
+      <c r="L39" s="28"/>
+      <c r="M39" s="28"/>
+      <c r="N39" s="28"/>
+      <c r="O39" s="28"/>
+      <c r="P39" s="35" t="s">
         <v>87</v>
       </c>
-      <c r="Q38" s="60"/>
-      <c r="R38" s="60"/>
-      <c r="S38" s="61"/>
-    </row>
-    <row r="39" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B39" s="38"/>
-      <c r="C39" s="39"/>
-      <c r="D39" s="38"/>
-      <c r="E39" s="43"/>
-      <c r="F39" s="5" t="s">
+      <c r="Q39" s="48"/>
+      <c r="R39" s="48"/>
+      <c r="S39" s="49"/>
+    </row>
+    <row r="40" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B40" s="31"/>
+      <c r="C40" s="32"/>
+      <c r="D40" s="31"/>
+      <c r="E40" s="34"/>
+      <c r="F40" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="G39" s="6"/>
-      <c r="H39" s="32" t="s">
+      <c r="G40" s="6"/>
+      <c r="H40" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="I39" s="32"/>
-      <c r="J39" s="32"/>
-      <c r="K39" s="32"/>
-      <c r="L39" s="32"/>
-      <c r="M39" s="32"/>
-      <c r="N39" s="32"/>
-      <c r="O39" s="32"/>
-      <c r="P39" s="66"/>
-      <c r="Q39" s="67"/>
-      <c r="R39" s="67"/>
-      <c r="S39" s="68"/>
-    </row>
-    <row r="40" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B40" s="38"/>
-      <c r="C40" s="39"/>
-      <c r="D40" s="38"/>
-      <c r="E40" s="43"/>
-      <c r="F40" s="5" t="s">
+      <c r="I40" s="28"/>
+      <c r="J40" s="28"/>
+      <c r="K40" s="28"/>
+      <c r="L40" s="28"/>
+      <c r="M40" s="28"/>
+      <c r="N40" s="28"/>
+      <c r="O40" s="28"/>
+      <c r="P40" s="53"/>
+      <c r="Q40" s="54"/>
+      <c r="R40" s="54"/>
+      <c r="S40" s="55"/>
+    </row>
+    <row r="41" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B41" s="31"/>
+      <c r="C41" s="32"/>
+      <c r="D41" s="31"/>
+      <c r="E41" s="34"/>
+      <c r="F41" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="G40" s="6"/>
-      <c r="H40" s="32" t="s">
+      <c r="G41" s="6"/>
+      <c r="H41" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="I40" s="32"/>
-      <c r="J40" s="32"/>
-      <c r="K40" s="32"/>
-      <c r="L40" s="32"/>
-      <c r="M40" s="32"/>
-      <c r="N40" s="32"/>
-      <c r="O40" s="32"/>
-      <c r="P40" s="66"/>
-      <c r="Q40" s="67"/>
-      <c r="R40" s="67"/>
-      <c r="S40" s="68"/>
-    </row>
-    <row r="41" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B41" s="38"/>
-      <c r="C41" s="39"/>
-      <c r="D41" s="38"/>
-      <c r="E41" s="43"/>
-      <c r="F41" s="5" t="s">
+      <c r="I41" s="28"/>
+      <c r="J41" s="28"/>
+      <c r="K41" s="28"/>
+      <c r="L41" s="28"/>
+      <c r="M41" s="28"/>
+      <c r="N41" s="28"/>
+      <c r="O41" s="28"/>
+      <c r="P41" s="53"/>
+      <c r="Q41" s="54"/>
+      <c r="R41" s="54"/>
+      <c r="S41" s="55"/>
+    </row>
+    <row r="42" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B42" s="31"/>
+      <c r="C42" s="32"/>
+      <c r="D42" s="31"/>
+      <c r="E42" s="34"/>
+      <c r="F42" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="G41" s="6"/>
-      <c r="H41" s="32" t="s">
+      <c r="G42" s="6"/>
+      <c r="H42" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="I41" s="32"/>
-      <c r="J41" s="32"/>
-      <c r="K41" s="32"/>
-      <c r="L41" s="32"/>
-      <c r="M41" s="32"/>
-      <c r="N41" s="32"/>
-      <c r="O41" s="32"/>
-      <c r="P41" s="66"/>
-      <c r="Q41" s="67"/>
-      <c r="R41" s="67"/>
-      <c r="S41" s="68"/>
-    </row>
-    <row r="42" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B42" s="38"/>
-      <c r="C42" s="39"/>
-      <c r="D42" s="38"/>
-      <c r="E42" s="43"/>
-      <c r="F42" s="5" t="s">
+      <c r="I42" s="28"/>
+      <c r="J42" s="28"/>
+      <c r="K42" s="28"/>
+      <c r="L42" s="28"/>
+      <c r="M42" s="28"/>
+      <c r="N42" s="28"/>
+      <c r="O42" s="28"/>
+      <c r="P42" s="53"/>
+      <c r="Q42" s="54"/>
+      <c r="R42" s="54"/>
+      <c r="S42" s="55"/>
+    </row>
+    <row r="43" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B43" s="31"/>
+      <c r="C43" s="32"/>
+      <c r="D43" s="31"/>
+      <c r="E43" s="34"/>
+      <c r="F43" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="G42" s="6"/>
-      <c r="H42" s="32" t="s">
+      <c r="G43" s="6"/>
+      <c r="H43" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="I42" s="32"/>
-      <c r="J42" s="32"/>
-      <c r="K42" s="32"/>
-      <c r="L42" s="32"/>
-      <c r="M42" s="32"/>
-      <c r="N42" s="32"/>
-      <c r="O42" s="32"/>
-      <c r="P42" s="66"/>
-      <c r="Q42" s="67"/>
-      <c r="R42" s="67"/>
-      <c r="S42" s="68"/>
-    </row>
-    <row r="43" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B43" s="38"/>
-      <c r="C43" s="39"/>
-      <c r="D43" s="38"/>
-      <c r="E43" s="43"/>
-      <c r="F43" s="5" t="s">
+      <c r="I43" s="28"/>
+      <c r="J43" s="28"/>
+      <c r="K43" s="28"/>
+      <c r="L43" s="28"/>
+      <c r="M43" s="28"/>
+      <c r="N43" s="28"/>
+      <c r="O43" s="28"/>
+      <c r="P43" s="53"/>
+      <c r="Q43" s="54"/>
+      <c r="R43" s="54"/>
+      <c r="S43" s="55"/>
+    </row>
+    <row r="44" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B44" s="31"/>
+      <c r="C44" s="32"/>
+      <c r="D44" s="31"/>
+      <c r="E44" s="34"/>
+      <c r="F44" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="G43" s="6"/>
-      <c r="H43" s="32" t="s">
+      <c r="G44" s="6"/>
+      <c r="H44" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="I43" s="32"/>
-      <c r="J43" s="32"/>
-      <c r="K43" s="32"/>
-      <c r="L43" s="32"/>
-      <c r="M43" s="32"/>
-      <c r="N43" s="32"/>
-      <c r="O43" s="32"/>
-      <c r="P43" s="66"/>
-      <c r="Q43" s="67"/>
-      <c r="R43" s="67"/>
-      <c r="S43" s="68"/>
-    </row>
-    <row r="44" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B44" s="38"/>
-      <c r="C44" s="39"/>
-      <c r="D44" s="38"/>
-      <c r="E44" s="43"/>
-      <c r="F44" s="5" t="s">
+      <c r="I44" s="28"/>
+      <c r="J44" s="28"/>
+      <c r="K44" s="28"/>
+      <c r="L44" s="28"/>
+      <c r="M44" s="28"/>
+      <c r="N44" s="28"/>
+      <c r="O44" s="28"/>
+      <c r="P44" s="53"/>
+      <c r="Q44" s="54"/>
+      <c r="R44" s="54"/>
+      <c r="S44" s="55"/>
+    </row>
+    <row r="45" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B45" s="31"/>
+      <c r="C45" s="32"/>
+      <c r="D45" s="31"/>
+      <c r="E45" s="34"/>
+      <c r="F45" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="G44" s="6"/>
-      <c r="H44" s="32" t="s">
+      <c r="G45" s="6"/>
+      <c r="H45" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="I44" s="32"/>
-      <c r="J44" s="32"/>
-      <c r="K44" s="32"/>
-      <c r="L44" s="32"/>
-      <c r="M44" s="32"/>
-      <c r="N44" s="32"/>
-      <c r="O44" s="32"/>
-      <c r="P44" s="66"/>
-      <c r="Q44" s="67"/>
-      <c r="R44" s="67"/>
-      <c r="S44" s="68"/>
-    </row>
-    <row r="45" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B45" s="38"/>
-      <c r="C45" s="39"/>
-      <c r="D45" s="38"/>
-      <c r="E45" s="43"/>
-      <c r="F45" s="5" t="s">
+      <c r="I45" s="28"/>
+      <c r="J45" s="28"/>
+      <c r="K45" s="28"/>
+      <c r="L45" s="28"/>
+      <c r="M45" s="28"/>
+      <c r="N45" s="28"/>
+      <c r="O45" s="28"/>
+      <c r="P45" s="53"/>
+      <c r="Q45" s="54"/>
+      <c r="R45" s="54"/>
+      <c r="S45" s="55"/>
+    </row>
+    <row r="46" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B46" s="31"/>
+      <c r="C46" s="32"/>
+      <c r="D46" s="31"/>
+      <c r="E46" s="34"/>
+      <c r="F46" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="G45" s="6"/>
-      <c r="H45" s="32" t="s">
+      <c r="G46" s="6"/>
+      <c r="H46" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="I45" s="32"/>
-      <c r="J45" s="32"/>
-      <c r="K45" s="32"/>
-      <c r="L45" s="32"/>
-      <c r="M45" s="32"/>
-      <c r="N45" s="32"/>
-      <c r="O45" s="32"/>
-      <c r="P45" s="66"/>
-      <c r="Q45" s="67"/>
-      <c r="R45" s="67"/>
-      <c r="S45" s="68"/>
-    </row>
-    <row r="46" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B46" s="38"/>
-      <c r="C46" s="39"/>
-      <c r="D46" s="38"/>
-      <c r="E46" s="43"/>
-      <c r="F46" s="5" t="s">
+      <c r="I46" s="28"/>
+      <c r="J46" s="28"/>
+      <c r="K46" s="28"/>
+      <c r="L46" s="28"/>
+      <c r="M46" s="28"/>
+      <c r="N46" s="28"/>
+      <c r="O46" s="28"/>
+      <c r="P46" s="53"/>
+      <c r="Q46" s="54"/>
+      <c r="R46" s="54"/>
+      <c r="S46" s="55"/>
+    </row>
+    <row r="47" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B47" s="31"/>
+      <c r="C47" s="32"/>
+      <c r="D47" s="31"/>
+      <c r="E47" s="34"/>
+      <c r="F47" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="G46" s="6"/>
-      <c r="H46" s="32" t="s">
+      <c r="G47" s="6"/>
+      <c r="H47" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="I46" s="32"/>
-      <c r="J46" s="32"/>
-      <c r="K46" s="32"/>
-      <c r="L46" s="32"/>
-      <c r="M46" s="32"/>
-      <c r="N46" s="32"/>
-      <c r="O46" s="32"/>
-      <c r="P46" s="66"/>
-      <c r="Q46" s="67"/>
-      <c r="R46" s="67"/>
-      <c r="S46" s="68"/>
-    </row>
-    <row r="47" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B47" s="38"/>
-      <c r="C47" s="39"/>
-      <c r="D47" s="38"/>
-      <c r="E47" s="43"/>
-      <c r="F47" s="11">
-        <v>0</v>
-      </c>
-      <c r="G47" s="6"/>
-      <c r="H47" s="32" t="s">
+      <c r="I47" s="28"/>
+      <c r="J47" s="28"/>
+      <c r="K47" s="28"/>
+      <c r="L47" s="28"/>
+      <c r="M47" s="28"/>
+      <c r="N47" s="28"/>
+      <c r="O47" s="28"/>
+      <c r="P47" s="53"/>
+      <c r="Q47" s="54"/>
+      <c r="R47" s="54"/>
+      <c r="S47" s="55"/>
+    </row>
+    <row r="48" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B48" s="31"/>
+      <c r="C48" s="32"/>
+      <c r="D48" s="31"/>
+      <c r="E48" s="34"/>
+      <c r="F48" s="11">
+        <v>0</v>
+      </c>
+      <c r="G48" s="6"/>
+      <c r="H48" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="I47" s="32"/>
-      <c r="J47" s="32"/>
-      <c r="K47" s="32"/>
-      <c r="L47" s="32"/>
-      <c r="M47" s="32"/>
-      <c r="N47" s="32"/>
-      <c r="O47" s="32"/>
-      <c r="P47" s="66"/>
-      <c r="Q47" s="67"/>
-      <c r="R47" s="67"/>
-      <c r="S47" s="68"/>
-    </row>
-    <row r="48" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B48" s="36" t="s">
+      <c r="I48" s="28"/>
+      <c r="J48" s="28"/>
+      <c r="K48" s="28"/>
+      <c r="L48" s="28"/>
+      <c r="M48" s="28"/>
+      <c r="N48" s="28"/>
+      <c r="O48" s="28"/>
+      <c r="P48" s="53"/>
+      <c r="Q48" s="54"/>
+      <c r="R48" s="54"/>
+      <c r="S48" s="55"/>
+    </row>
+    <row r="49" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B49" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="C48" s="37"/>
-      <c r="D48" s="36" t="s">
+      <c r="C49" s="30"/>
+      <c r="D49" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="E48" s="42"/>
-      <c r="F48" s="12" t="s">
+      <c r="E49" s="33"/>
+      <c r="F49" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="G48" s="13"/>
-      <c r="H48" s="45" t="s">
+      <c r="G49" s="13"/>
+      <c r="H49" s="44" t="s">
         <v>106</v>
       </c>
-      <c r="I48" s="46"/>
-      <c r="J48" s="46"/>
-      <c r="K48" s="46"/>
-      <c r="L48" s="46"/>
-      <c r="M48" s="46"/>
-      <c r="N48" s="46"/>
-      <c r="O48" s="47"/>
-      <c r="P48" s="59" t="s">
+      <c r="I49" s="36"/>
+      <c r="J49" s="36"/>
+      <c r="K49" s="36"/>
+      <c r="L49" s="36"/>
+      <c r="M49" s="36"/>
+      <c r="N49" s="36"/>
+      <c r="O49" s="37"/>
+      <c r="P49" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="Q48" s="46"/>
-      <c r="R48" s="46"/>
-      <c r="S48" s="47"/>
-    </row>
-    <row r="49" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B49" s="40"/>
-      <c r="C49" s="41"/>
-      <c r="D49" s="40"/>
-      <c r="E49" s="44"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="15"/>
-      <c r="H49" s="51"/>
-      <c r="I49" s="52"/>
-      <c r="J49" s="52"/>
-      <c r="K49" s="52"/>
-      <c r="L49" s="52"/>
-      <c r="M49" s="52"/>
-      <c r="N49" s="52"/>
-      <c r="O49" s="53"/>
-      <c r="P49" s="51"/>
-      <c r="Q49" s="52"/>
-      <c r="R49" s="52"/>
-      <c r="S49" s="53"/>
+      <c r="Q49" s="36"/>
+      <c r="R49" s="36"/>
+      <c r="S49" s="37"/>
     </row>
     <row r="50" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B50" s="56" t="s">
+      <c r="B50" s="41"/>
+      <c r="C50" s="42"/>
+      <c r="D50" s="41"/>
+      <c r="E50" s="43"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="15"/>
+      <c r="H50" s="45"/>
+      <c r="I50" s="46"/>
+      <c r="J50" s="46"/>
+      <c r="K50" s="46"/>
+      <c r="L50" s="46"/>
+      <c r="M50" s="46"/>
+      <c r="N50" s="46"/>
+      <c r="O50" s="47"/>
+      <c r="P50" s="45"/>
+      <c r="Q50" s="46"/>
+      <c r="R50" s="46"/>
+      <c r="S50" s="47"/>
+    </row>
+    <row r="51" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B51" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="C50" s="56"/>
-      <c r="D50" s="56" t="s">
+      <c r="C51" s="26"/>
+      <c r="D51" s="26" t="s">
         <v>109</v>
       </c>
-      <c r="E50" s="29"/>
-      <c r="F50" s="5" t="s">
+      <c r="E51" s="27"/>
+      <c r="F51" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G50" s="6"/>
-      <c r="H50" s="32" t="s">
+      <c r="G51" s="6"/>
+      <c r="H51" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="I50" s="32"/>
-      <c r="J50" s="32"/>
-      <c r="K50" s="32"/>
-      <c r="L50" s="32"/>
-      <c r="M50" s="32"/>
-      <c r="N50" s="32"/>
-      <c r="O50" s="32"/>
-      <c r="P50" s="32"/>
-      <c r="Q50" s="32"/>
-      <c r="R50" s="32"/>
-      <c r="S50" s="32"/>
-    </row>
-    <row r="51" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B51" s="36" t="s">
+      <c r="I51" s="28"/>
+      <c r="J51" s="28"/>
+      <c r="K51" s="28"/>
+      <c r="L51" s="28"/>
+      <c r="M51" s="28"/>
+      <c r="N51" s="28"/>
+      <c r="O51" s="28"/>
+      <c r="P51" s="28"/>
+      <c r="Q51" s="28"/>
+      <c r="R51" s="28"/>
+      <c r="S51" s="28"/>
+    </row>
+    <row r="52" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B52" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="C51" s="37"/>
-      <c r="D51" s="36" t="s">
+      <c r="C52" s="30"/>
+      <c r="D52" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="E51" s="42"/>
-      <c r="F51" s="5" t="s">
+      <c r="E52" s="33"/>
+      <c r="F52" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="G51" s="6"/>
-      <c r="H51" s="32" t="s">
+      <c r="G52" s="6"/>
+      <c r="H52" s="28" t="s">
         <v>114</v>
       </c>
-      <c r="I51" s="32"/>
-      <c r="J51" s="32"/>
-      <c r="K51" s="32"/>
-      <c r="L51" s="32"/>
-      <c r="M51" s="32"/>
-      <c r="N51" s="32"/>
-      <c r="O51" s="32"/>
-      <c r="P51" s="45"/>
-      <c r="Q51" s="46"/>
-      <c r="R51" s="46"/>
-      <c r="S51" s="47"/>
-    </row>
-    <row r="52" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B52" s="38"/>
-      <c r="C52" s="39"/>
-      <c r="D52" s="38"/>
-      <c r="E52" s="43"/>
-      <c r="F52" s="5" t="s">
+      <c r="I52" s="28"/>
+      <c r="J52" s="28"/>
+      <c r="K52" s="28"/>
+      <c r="L52" s="28"/>
+      <c r="M52" s="28"/>
+      <c r="N52" s="28"/>
+      <c r="O52" s="28"/>
+      <c r="P52" s="44"/>
+      <c r="Q52" s="36"/>
+      <c r="R52" s="36"/>
+      <c r="S52" s="37"/>
+    </row>
+    <row r="53" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B53" s="31"/>
+      <c r="C53" s="32"/>
+      <c r="D53" s="31"/>
+      <c r="E53" s="34"/>
+      <c r="F53" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="G52" s="6"/>
-      <c r="H52" s="32" t="s">
+      <c r="G53" s="6"/>
+      <c r="H53" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="I52" s="32"/>
-      <c r="J52" s="32"/>
-      <c r="K52" s="32"/>
-      <c r="L52" s="32"/>
-      <c r="M52" s="32"/>
-      <c r="N52" s="32"/>
-      <c r="O52" s="32"/>
-      <c r="P52" s="48"/>
-      <c r="Q52" s="49"/>
-      <c r="R52" s="49"/>
-      <c r="S52" s="50"/>
-    </row>
-    <row r="53" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B53" s="40"/>
-      <c r="C53" s="41"/>
-      <c r="D53" s="40"/>
-      <c r="E53" s="44"/>
-      <c r="F53" s="11">
-        <v>0</v>
-      </c>
-      <c r="G53" s="6"/>
-      <c r="H53" s="32" t="s">
+      <c r="I53" s="28"/>
+      <c r="J53" s="28"/>
+      <c r="K53" s="28"/>
+      <c r="L53" s="28"/>
+      <c r="M53" s="28"/>
+      <c r="N53" s="28"/>
+      <c r="O53" s="28"/>
+      <c r="P53" s="38"/>
+      <c r="Q53" s="39"/>
+      <c r="R53" s="39"/>
+      <c r="S53" s="40"/>
+    </row>
+    <row r="54" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B54" s="41"/>
+      <c r="C54" s="42"/>
+      <c r="D54" s="41"/>
+      <c r="E54" s="43"/>
+      <c r="F54" s="11">
+        <v>0</v>
+      </c>
+      <c r="G54" s="6"/>
+      <c r="H54" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="I53" s="32"/>
-      <c r="J53" s="32"/>
-      <c r="K53" s="32"/>
-      <c r="L53" s="32"/>
-      <c r="M53" s="32"/>
-      <c r="N53" s="32"/>
-      <c r="O53" s="32"/>
-      <c r="P53" s="51"/>
-      <c r="Q53" s="52"/>
-      <c r="R53" s="52"/>
-      <c r="S53" s="53"/>
-    </row>
-    <row r="54" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B54" s="56" t="s">
+      <c r="I54" s="28"/>
+      <c r="J54" s="28"/>
+      <c r="K54" s="28"/>
+      <c r="L54" s="28"/>
+      <c r="M54" s="28"/>
+      <c r="N54" s="28"/>
+      <c r="O54" s="28"/>
+      <c r="P54" s="45"/>
+      <c r="Q54" s="46"/>
+      <c r="R54" s="46"/>
+      <c r="S54" s="47"/>
+    </row>
+    <row r="55" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B55" s="26" t="s">
         <v>117</v>
       </c>
-      <c r="C54" s="56"/>
-      <c r="D54" s="56" t="s">
+      <c r="C55" s="26"/>
+      <c r="D55" s="26" t="s">
         <v>118</v>
       </c>
-      <c r="E54" s="29"/>
-      <c r="F54" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G54" s="6"/>
-      <c r="H54" s="32" t="s">
-        <v>119</v>
-      </c>
-      <c r="I54" s="32"/>
-      <c r="J54" s="32"/>
-      <c r="K54" s="32"/>
-      <c r="L54" s="32"/>
-      <c r="M54" s="32"/>
-      <c r="N54" s="32"/>
-      <c r="O54" s="32"/>
-      <c r="P54" s="32" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q54" s="32"/>
-      <c r="R54" s="32"/>
-      <c r="S54" s="32"/>
-    </row>
-    <row r="55" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B55" s="56" t="s">
-        <v>121</v>
-      </c>
-      <c r="C55" s="56"/>
-      <c r="D55" s="56" t="s">
-        <v>122</v>
-      </c>
-      <c r="E55" s="29"/>
+      <c r="E55" s="27"/>
       <c r="F55" s="5" t="s">
         <v>8</v>
       </c>
       <c r="G55" s="6"/>
-      <c r="H55" s="32" t="s">
-        <v>123</v>
-      </c>
-      <c r="I55" s="32"/>
-      <c r="J55" s="32"/>
-      <c r="K55" s="32"/>
-      <c r="L55" s="32"/>
-      <c r="M55" s="32"/>
-      <c r="N55" s="32"/>
-      <c r="O55" s="32"/>
-      <c r="P55" s="32" t="s">
+      <c r="H55" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="I55" s="28"/>
+      <c r="J55" s="28"/>
+      <c r="K55" s="28"/>
+      <c r="L55" s="28"/>
+      <c r="M55" s="28"/>
+      <c r="N55" s="28"/>
+      <c r="O55" s="28"/>
+      <c r="P55" s="28" t="s">
         <v>120</v>
       </c>
-      <c r="Q55" s="32"/>
-      <c r="R55" s="32"/>
-      <c r="S55" s="32"/>
+      <c r="Q55" s="28"/>
+      <c r="R55" s="28"/>
+      <c r="S55" s="28"/>
     </row>
     <row r="56" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B56" s="56" t="s">
-        <v>124</v>
-      </c>
-      <c r="C56" s="56"/>
-      <c r="D56" s="56" t="s">
-        <v>125</v>
-      </c>
-      <c r="E56" s="29"/>
+      <c r="B56" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="C56" s="26"/>
+      <c r="D56" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="E56" s="27"/>
       <c r="F56" s="5" t="s">
         <v>8</v>
       </c>
       <c r="G56" s="6"/>
-      <c r="H56" s="32" t="s">
+      <c r="H56" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="I56" s="28"/>
+      <c r="J56" s="28"/>
+      <c r="K56" s="28"/>
+      <c r="L56" s="28"/>
+      <c r="M56" s="28"/>
+      <c r="N56" s="28"/>
+      <c r="O56" s="28"/>
+      <c r="P56" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q56" s="28"/>
+      <c r="R56" s="28"/>
+      <c r="S56" s="28"/>
+    </row>
+    <row r="57" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B57" s="26" t="s">
+        <v>124</v>
+      </c>
+      <c r="C57" s="26"/>
+      <c r="D57" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="E57" s="27"/>
+      <c r="F57" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G57" s="6"/>
+      <c r="H57" s="28" t="s">
         <v>126</v>
       </c>
-      <c r="I56" s="32"/>
-      <c r="J56" s="32"/>
-      <c r="K56" s="32"/>
-      <c r="L56" s="32"/>
-      <c r="M56" s="32"/>
-      <c r="N56" s="32"/>
-      <c r="O56" s="32"/>
-      <c r="P56" s="32" t="s">
+      <c r="I57" s="28"/>
+      <c r="J57" s="28"/>
+      <c r="K57" s="28"/>
+      <c r="L57" s="28"/>
+      <c r="M57" s="28"/>
+      <c r="N57" s="28"/>
+      <c r="O57" s="28"/>
+      <c r="P57" s="28" t="s">
         <v>127</v>
       </c>
-      <c r="Q56" s="32"/>
-      <c r="R56" s="32"/>
-      <c r="S56" s="32"/>
-    </row>
-    <row r="57" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B57" s="56" t="s">
+      <c r="Q57" s="28"/>
+      <c r="R57" s="28"/>
+      <c r="S57" s="28"/>
+    </row>
+    <row r="58" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B58" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="C57" s="56"/>
-      <c r="D57" s="56" t="s">
+      <c r="C58" s="26"/>
+      <c r="D58" s="26" t="s">
         <v>129</v>
       </c>
-      <c r="E57" s="29"/>
-      <c r="F57" s="5" t="s">
+      <c r="E58" s="27"/>
+      <c r="F58" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G57" s="6"/>
-      <c r="H57" s="32" t="s">
+      <c r="G58" s="6"/>
+      <c r="H58" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="I57" s="32"/>
-      <c r="J57" s="32"/>
-      <c r="K57" s="32"/>
-      <c r="L57" s="32"/>
-      <c r="M57" s="32"/>
-      <c r="N57" s="32"/>
-      <c r="O57" s="32"/>
-      <c r="P57" s="32"/>
-      <c r="Q57" s="32"/>
-      <c r="R57" s="32"/>
-      <c r="S57" s="32"/>
-    </row>
-    <row r="58" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B58" s="36" t="s">
+      <c r="I58" s="28"/>
+      <c r="J58" s="28"/>
+      <c r="K58" s="28"/>
+      <c r="L58" s="28"/>
+      <c r="M58" s="28"/>
+      <c r="N58" s="28"/>
+      <c r="O58" s="28"/>
+      <c r="P58" s="28"/>
+      <c r="Q58" s="28"/>
+      <c r="R58" s="28"/>
+      <c r="S58" s="28"/>
+    </row>
+    <row r="59" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B59" s="29" t="s">
         <v>131</v>
       </c>
-      <c r="C58" s="37"/>
-      <c r="D58" s="36" t="s">
+      <c r="C59" s="30"/>
+      <c r="D59" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="E58" s="42"/>
-      <c r="F58" s="12" t="s">
+      <c r="E59" s="33"/>
+      <c r="F59" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="G58" s="13"/>
-      <c r="H58" s="45" t="s">
+      <c r="G59" s="13"/>
+      <c r="H59" s="44" t="s">
         <v>133</v>
       </c>
-      <c r="I58" s="46"/>
-      <c r="J58" s="46"/>
-      <c r="K58" s="46"/>
-      <c r="L58" s="46"/>
-      <c r="M58" s="46"/>
-      <c r="N58" s="46"/>
-      <c r="O58" s="47"/>
-      <c r="P58" s="59" t="s">
+      <c r="I59" s="36"/>
+      <c r="J59" s="36"/>
+      <c r="K59" s="36"/>
+      <c r="L59" s="36"/>
+      <c r="M59" s="36"/>
+      <c r="N59" s="36"/>
+      <c r="O59" s="37"/>
+      <c r="P59" s="35" t="s">
         <v>134</v>
       </c>
-      <c r="Q58" s="46"/>
-      <c r="R58" s="46"/>
-      <c r="S58" s="47"/>
-    </row>
-    <row r="59" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B59" s="40"/>
-      <c r="C59" s="41"/>
-      <c r="D59" s="40"/>
-      <c r="E59" s="44"/>
-      <c r="F59" s="14"/>
-      <c r="G59" s="15"/>
-      <c r="H59" s="51"/>
-      <c r="I59" s="52"/>
-      <c r="J59" s="52"/>
-      <c r="K59" s="52"/>
-      <c r="L59" s="52"/>
-      <c r="M59" s="52"/>
-      <c r="N59" s="52"/>
-      <c r="O59" s="53"/>
-      <c r="P59" s="51"/>
-      <c r="Q59" s="52"/>
-      <c r="R59" s="52"/>
-      <c r="S59" s="53"/>
+      <c r="Q59" s="36"/>
+      <c r="R59" s="36"/>
+      <c r="S59" s="37"/>
     </row>
     <row r="60" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B60" s="36" t="s">
-        <v>135</v>
-      </c>
-      <c r="C60" s="37"/>
-      <c r="D60" s="36" t="s">
-        <v>136</v>
-      </c>
-      <c r="E60" s="42"/>
-      <c r="F60" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="G60" s="6"/>
-      <c r="H60" s="32" t="s">
-        <v>137</v>
-      </c>
-      <c r="I60" s="32"/>
-      <c r="J60" s="32"/>
-      <c r="K60" s="32"/>
-      <c r="L60" s="32"/>
-      <c r="M60" s="32"/>
-      <c r="N60" s="32"/>
-      <c r="O60" s="32"/>
-      <c r="P60" s="59" t="s">
-        <v>138</v>
-      </c>
+      <c r="B60" s="41"/>
+      <c r="C60" s="42"/>
+      <c r="D60" s="41"/>
+      <c r="E60" s="43"/>
+      <c r="F60" s="14"/>
+      <c r="G60" s="15"/>
+      <c r="H60" s="45"/>
+      <c r="I60" s="46"/>
+      <c r="J60" s="46"/>
+      <c r="K60" s="46"/>
+      <c r="L60" s="46"/>
+      <c r="M60" s="46"/>
+      <c r="N60" s="46"/>
+      <c r="O60" s="47"/>
+      <c r="P60" s="45"/>
       <c r="Q60" s="46"/>
       <c r="R60" s="46"/>
       <c r="S60" s="47"/>
     </row>
     <row r="61" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B61" s="40"/>
-      <c r="C61" s="41"/>
-      <c r="D61" s="40"/>
-      <c r="E61" s="44"/>
+      <c r="B61" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="C61" s="30"/>
+      <c r="D61" s="29" t="s">
+        <v>136</v>
+      </c>
+      <c r="E61" s="33"/>
       <c r="F61" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G61" s="6"/>
-      <c r="H61" s="32" t="s">
+      <c r="H61" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="I61" s="28"/>
+      <c r="J61" s="28"/>
+      <c r="K61" s="28"/>
+      <c r="L61" s="28"/>
+      <c r="M61" s="28"/>
+      <c r="N61" s="28"/>
+      <c r="O61" s="28"/>
+      <c r="P61" s="35" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q61" s="36"/>
+      <c r="R61" s="36"/>
+      <c r="S61" s="37"/>
+    </row>
+    <row r="62" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B62" s="41"/>
+      <c r="C62" s="42"/>
+      <c r="D62" s="41"/>
+      <c r="E62" s="43"/>
+      <c r="F62" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="G62" s="6"/>
+      <c r="H62" s="28" t="s">
         <v>139</v>
       </c>
-      <c r="I61" s="32"/>
-      <c r="J61" s="32"/>
-      <c r="K61" s="32"/>
-      <c r="L61" s="32"/>
-      <c r="M61" s="32"/>
-      <c r="N61" s="32"/>
-      <c r="O61" s="32"/>
-      <c r="P61" s="51"/>
-      <c r="Q61" s="52"/>
-      <c r="R61" s="52"/>
-      <c r="S61" s="53"/>
-    </row>
-    <row r="62" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B62" s="36" t="s">
-        <v>140</v>
-      </c>
-      <c r="C62" s="37"/>
-      <c r="D62" s="36" t="s">
-        <v>141</v>
-      </c>
-      <c r="E62" s="42"/>
-      <c r="F62" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="G62" s="6"/>
-      <c r="H62" s="32" t="s">
-        <v>142</v>
-      </c>
-      <c r="I62" s="32"/>
-      <c r="J62" s="32"/>
-      <c r="K62" s="32"/>
-      <c r="L62" s="32"/>
-      <c r="M62" s="32"/>
-      <c r="N62" s="32"/>
-      <c r="O62" s="32"/>
-      <c r="P62" s="59"/>
+      <c r="I62" s="28"/>
+      <c r="J62" s="28"/>
+      <c r="K62" s="28"/>
+      <c r="L62" s="28"/>
+      <c r="M62" s="28"/>
+      <c r="N62" s="28"/>
+      <c r="O62" s="28"/>
+      <c r="P62" s="45"/>
       <c r="Q62" s="46"/>
       <c r="R62" s="46"/>
       <c r="S62" s="47"/>
     </row>
     <row r="63" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B63" s="40"/>
-      <c r="C63" s="41"/>
-      <c r="D63" s="40"/>
-      <c r="E63" s="44"/>
+      <c r="B63" s="29" t="s">
+        <v>140</v>
+      </c>
+      <c r="C63" s="30"/>
+      <c r="D63" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="E63" s="33"/>
       <c r="F63" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G63" s="6"/>
-      <c r="H63" s="32" t="s">
+      <c r="H63" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="I63" s="28"/>
+      <c r="J63" s="28"/>
+      <c r="K63" s="28"/>
+      <c r="L63" s="28"/>
+      <c r="M63" s="28"/>
+      <c r="N63" s="28"/>
+      <c r="O63" s="28"/>
+      <c r="P63" s="35"/>
+      <c r="Q63" s="36"/>
+      <c r="R63" s="36"/>
+      <c r="S63" s="37"/>
+    </row>
+    <row r="64" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B64" s="41"/>
+      <c r="C64" s="42"/>
+      <c r="D64" s="41"/>
+      <c r="E64" s="43"/>
+      <c r="F64" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="G64" s="6"/>
+      <c r="H64" s="28" t="s">
         <v>143</v>
       </c>
-      <c r="I63" s="32"/>
-      <c r="J63" s="32"/>
-      <c r="K63" s="32"/>
-      <c r="L63" s="32"/>
-      <c r="M63" s="32"/>
-      <c r="N63" s="32"/>
-      <c r="O63" s="32"/>
-      <c r="P63" s="69"/>
-      <c r="Q63" s="32"/>
-      <c r="R63" s="32"/>
-      <c r="S63" s="32"/>
-    </row>
-    <row r="67" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B67" s="2" t="s">
+      <c r="I64" s="28"/>
+      <c r="J64" s="28"/>
+      <c r="K64" s="28"/>
+      <c r="L64" s="28"/>
+      <c r="M64" s="28"/>
+      <c r="N64" s="28"/>
+      <c r="O64" s="28"/>
+      <c r="P64" s="60"/>
+      <c r="Q64" s="28"/>
+      <c r="R64" s="28"/>
+      <c r="S64" s="28"/>
+    </row>
+    <row r="68" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B68" s="2" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="68" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B68" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="C68" s="26"/>
-      <c r="D68" s="26" t="s">
+    <row r="69" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B69" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="C69" s="56"/>
+      <c r="D69" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="E68" s="27"/>
-      <c r="F68" s="54" t="s">
+      <c r="E69" s="57"/>
+      <c r="F69" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="G68" s="55"/>
-      <c r="H68" s="26" t="s">
+      <c r="G69" s="59"/>
+      <c r="H69" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="I68" s="26"/>
-      <c r="J68" s="26"/>
-      <c r="K68" s="26"/>
-      <c r="L68" s="26"/>
-      <c r="M68" s="26"/>
-      <c r="N68" s="26"/>
-      <c r="O68" s="26"/>
-      <c r="P68" s="26" t="s">
+      <c r="I69" s="56"/>
+      <c r="J69" s="56"/>
+      <c r="K69" s="56"/>
+      <c r="L69" s="56"/>
+      <c r="M69" s="56"/>
+      <c r="N69" s="56"/>
+      <c r="O69" s="56"/>
+      <c r="P69" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="Q68" s="26"/>
-      <c r="R68" s="26"/>
-      <c r="S68" s="26"/>
-    </row>
-    <row r="69" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B69" s="36" t="s">
+      <c r="Q69" s="56"/>
+      <c r="R69" s="56"/>
+      <c r="S69" s="56"/>
+    </row>
+    <row r="70" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B70" s="29" t="s">
         <v>145</v>
       </c>
-      <c r="C69" s="37"/>
-      <c r="D69" s="36" t="s">
+      <c r="C70" s="30"/>
+      <c r="D70" s="29" t="s">
         <v>146</v>
       </c>
-      <c r="E69" s="42"/>
-      <c r="F69" s="5" t="s">
+      <c r="E70" s="33"/>
+      <c r="F70" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="G69" s="6"/>
-      <c r="H69" s="32" t="s">
+      <c r="G70" s="6"/>
+      <c r="H70" s="28" t="s">
         <v>148</v>
       </c>
-      <c r="I69" s="32"/>
-      <c r="J69" s="32"/>
-      <c r="K69" s="32"/>
-      <c r="L69" s="32"/>
-      <c r="M69" s="32"/>
-      <c r="N69" s="32"/>
-      <c r="O69" s="32"/>
-      <c r="P69" s="45"/>
-      <c r="Q69" s="46"/>
-      <c r="R69" s="46"/>
-      <c r="S69" s="47"/>
-    </row>
-    <row r="70" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B70" s="40"/>
-      <c r="C70" s="41"/>
-      <c r="D70" s="40"/>
-      <c r="E70" s="44"/>
-      <c r="F70" s="5" t="s">
+      <c r="I70" s="28"/>
+      <c r="J70" s="28"/>
+      <c r="K70" s="28"/>
+      <c r="L70" s="28"/>
+      <c r="M70" s="28"/>
+      <c r="N70" s="28"/>
+      <c r="O70" s="28"/>
+      <c r="P70" s="44"/>
+      <c r="Q70" s="36"/>
+      <c r="R70" s="36"/>
+      <c r="S70" s="37"/>
+    </row>
+    <row r="71" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B71" s="41"/>
+      <c r="C71" s="42"/>
+      <c r="D71" s="41"/>
+      <c r="E71" s="43"/>
+      <c r="F71" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="G70" s="6"/>
-      <c r="H70" s="32" t="s">
+      <c r="G71" s="6"/>
+      <c r="H71" s="28" t="s">
         <v>150</v>
       </c>
-      <c r="I70" s="32"/>
-      <c r="J70" s="32"/>
-      <c r="K70" s="32"/>
-      <c r="L70" s="32"/>
-      <c r="M70" s="32"/>
-      <c r="N70" s="32"/>
-      <c r="O70" s="32"/>
-      <c r="P70" s="51"/>
-      <c r="Q70" s="52"/>
-      <c r="R70" s="52"/>
-      <c r="S70" s="53"/>
-    </row>
-    <row r="71" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B71" s="36" t="s">
+      <c r="I71" s="28"/>
+      <c r="J71" s="28"/>
+      <c r="K71" s="28"/>
+      <c r="L71" s="28"/>
+      <c r="M71" s="28"/>
+      <c r="N71" s="28"/>
+      <c r="O71" s="28"/>
+      <c r="P71" s="45"/>
+      <c r="Q71" s="46"/>
+      <c r="R71" s="46"/>
+      <c r="S71" s="47"/>
+    </row>
+    <row r="72" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B72" s="29" t="s">
         <v>151</v>
       </c>
-      <c r="C71" s="37"/>
-      <c r="D71" s="36" t="s">
+      <c r="C72" s="30"/>
+      <c r="D72" s="29" t="s">
         <v>152</v>
       </c>
-      <c r="E71" s="42"/>
-      <c r="F71" s="5" t="s">
+      <c r="E72" s="33"/>
+      <c r="F72" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="G71" s="6"/>
-      <c r="H71" s="32" t="s">
+      <c r="G72" s="6"/>
+      <c r="H72" s="28" t="s">
         <v>154</v>
       </c>
-      <c r="I71" s="32"/>
-      <c r="J71" s="32"/>
-      <c r="K71" s="32"/>
-      <c r="L71" s="32"/>
-      <c r="M71" s="32"/>
-      <c r="N71" s="32"/>
-      <c r="O71" s="32"/>
-      <c r="P71" s="59"/>
-      <c r="Q71" s="60"/>
-      <c r="R71" s="60"/>
-      <c r="S71" s="61"/>
-    </row>
-    <row r="72" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B72" s="38"/>
-      <c r="C72" s="39"/>
-      <c r="D72" s="38"/>
-      <c r="E72" s="43"/>
-      <c r="F72" s="5" t="s">
+      <c r="I72" s="28"/>
+      <c r="J72" s="28"/>
+      <c r="K72" s="28"/>
+      <c r="L72" s="28"/>
+      <c r="M72" s="28"/>
+      <c r="N72" s="28"/>
+      <c r="O72" s="28"/>
+      <c r="P72" s="35"/>
+      <c r="Q72" s="48"/>
+      <c r="R72" s="48"/>
+      <c r="S72" s="49"/>
+    </row>
+    <row r="73" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B73" s="31"/>
+      <c r="C73" s="32"/>
+      <c r="D73" s="31"/>
+      <c r="E73" s="34"/>
+      <c r="F73" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="G72" s="6"/>
-      <c r="H72" s="32" t="s">
+      <c r="G73" s="6"/>
+      <c r="H73" s="28" t="s">
         <v>155</v>
       </c>
-      <c r="I72" s="32"/>
-      <c r="J72" s="32"/>
-      <c r="K72" s="32"/>
-      <c r="L72" s="32"/>
-      <c r="M72" s="32"/>
-      <c r="N72" s="32"/>
-      <c r="O72" s="32"/>
-      <c r="P72" s="66"/>
-      <c r="Q72" s="67"/>
-      <c r="R72" s="67"/>
-      <c r="S72" s="68"/>
-    </row>
-    <row r="73" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B73" s="38"/>
-      <c r="C73" s="39"/>
-      <c r="D73" s="38"/>
-      <c r="E73" s="43"/>
-      <c r="F73" s="5" t="s">
+      <c r="I73" s="28"/>
+      <c r="J73" s="28"/>
+      <c r="K73" s="28"/>
+      <c r="L73" s="28"/>
+      <c r="M73" s="28"/>
+      <c r="N73" s="28"/>
+      <c r="O73" s="28"/>
+      <c r="P73" s="53"/>
+      <c r="Q73" s="54"/>
+      <c r="R73" s="54"/>
+      <c r="S73" s="55"/>
+    </row>
+    <row r="74" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B74" s="31"/>
+      <c r="C74" s="32"/>
+      <c r="D74" s="31"/>
+      <c r="E74" s="34"/>
+      <c r="F74" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="G73" s="6"/>
-      <c r="H73" s="32" t="s">
+      <c r="G74" s="6"/>
+      <c r="H74" s="28" t="s">
         <v>157</v>
       </c>
-      <c r="I73" s="32"/>
-      <c r="J73" s="32"/>
-      <c r="K73" s="32"/>
-      <c r="L73" s="32"/>
-      <c r="M73" s="32"/>
-      <c r="N73" s="32"/>
-      <c r="O73" s="32"/>
-      <c r="P73" s="66"/>
-      <c r="Q73" s="67"/>
-      <c r="R73" s="67"/>
-      <c r="S73" s="68"/>
-    </row>
-    <row r="74" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B74" s="36" t="s">
+      <c r="I74" s="28"/>
+      <c r="J74" s="28"/>
+      <c r="K74" s="28"/>
+      <c r="L74" s="28"/>
+      <c r="M74" s="28"/>
+      <c r="N74" s="28"/>
+      <c r="O74" s="28"/>
+      <c r="P74" s="53"/>
+      <c r="Q74" s="54"/>
+      <c r="R74" s="54"/>
+      <c r="S74" s="55"/>
+    </row>
+    <row r="75" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B75" s="29" t="s">
         <v>158</v>
       </c>
-      <c r="C74" s="37"/>
-      <c r="D74" s="36" t="s">
+      <c r="C75" s="30"/>
+      <c r="D75" s="29" t="s">
         <v>159</v>
       </c>
-      <c r="E74" s="42"/>
-      <c r="F74" s="5" t="s">
+      <c r="E75" s="33"/>
+      <c r="F75" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G74" s="6"/>
-      <c r="H74" s="32" t="s">
+      <c r="G75" s="6"/>
+      <c r="H75" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="I74" s="32"/>
-      <c r="J74" s="32"/>
-      <c r="K74" s="32"/>
-      <c r="L74" s="32"/>
-      <c r="M74" s="32"/>
-      <c r="N74" s="32"/>
-      <c r="O74" s="32"/>
-      <c r="P74" s="45" t="s">
+      <c r="I75" s="28"/>
+      <c r="J75" s="28"/>
+      <c r="K75" s="28"/>
+      <c r="L75" s="28"/>
+      <c r="M75" s="28"/>
+      <c r="N75" s="28"/>
+      <c r="O75" s="28"/>
+      <c r="P75" s="44" t="s">
         <v>161</v>
       </c>
-      <c r="Q74" s="46"/>
-      <c r="R74" s="46"/>
-      <c r="S74" s="47"/>
-    </row>
-    <row r="75" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B75" s="36" t="s">
+      <c r="Q75" s="36"/>
+      <c r="R75" s="36"/>
+      <c r="S75" s="37"/>
+    </row>
+    <row r="76" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B76" s="29" t="s">
         <v>162</v>
       </c>
-      <c r="C75" s="37"/>
-      <c r="D75" s="36" t="s">
+      <c r="C76" s="30"/>
+      <c r="D76" s="29" t="s">
         <v>163</v>
       </c>
-      <c r="E75" s="42"/>
-      <c r="F75" s="5" t="s">
+      <c r="E76" s="33"/>
+      <c r="F76" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="G75" s="6"/>
-      <c r="H75" s="32" t="s">
+      <c r="G76" s="6"/>
+      <c r="H76" s="28" t="s">
         <v>164</v>
       </c>
-      <c r="I75" s="32"/>
-      <c r="J75" s="32"/>
-      <c r="K75" s="32"/>
-      <c r="L75" s="32"/>
-      <c r="M75" s="32"/>
-      <c r="N75" s="32"/>
-      <c r="O75" s="32"/>
-      <c r="P75" s="45"/>
-      <c r="Q75" s="46"/>
-      <c r="R75" s="46"/>
-      <c r="S75" s="47"/>
-    </row>
-    <row r="76" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B76" s="38"/>
-      <c r="C76" s="39"/>
-      <c r="D76" s="38"/>
-      <c r="E76" s="43"/>
-      <c r="F76" s="5" t="s">
+      <c r="I76" s="28"/>
+      <c r="J76" s="28"/>
+      <c r="K76" s="28"/>
+      <c r="L76" s="28"/>
+      <c r="M76" s="28"/>
+      <c r="N76" s="28"/>
+      <c r="O76" s="28"/>
+      <c r="P76" s="44"/>
+      <c r="Q76" s="36"/>
+      <c r="R76" s="36"/>
+      <c r="S76" s="37"/>
+    </row>
+    <row r="77" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B77" s="31"/>
+      <c r="C77" s="32"/>
+      <c r="D77" s="31"/>
+      <c r="E77" s="34"/>
+      <c r="F77" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="G76" s="6"/>
-      <c r="H76" s="32" t="s">
+      <c r="G77" s="6"/>
+      <c r="H77" s="28" t="s">
         <v>166</v>
       </c>
-      <c r="I76" s="32"/>
-      <c r="J76" s="32"/>
-      <c r="K76" s="32"/>
-      <c r="L76" s="32"/>
-      <c r="M76" s="32"/>
-      <c r="N76" s="32"/>
-      <c r="O76" s="32"/>
-      <c r="P76" s="48"/>
-      <c r="Q76" s="49"/>
-      <c r="R76" s="49"/>
-      <c r="S76" s="50"/>
-    </row>
-    <row r="77" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B77" s="40"/>
-      <c r="C77" s="41"/>
-      <c r="D77" s="40"/>
-      <c r="E77" s="44"/>
-      <c r="F77" s="11">
-        <v>0</v>
-      </c>
-      <c r="G77" s="6"/>
-      <c r="H77" s="32" t="s">
+      <c r="I77" s="28"/>
+      <c r="J77" s="28"/>
+      <c r="K77" s="28"/>
+      <c r="L77" s="28"/>
+      <c r="M77" s="28"/>
+      <c r="N77" s="28"/>
+      <c r="O77" s="28"/>
+      <c r="P77" s="38"/>
+      <c r="Q77" s="39"/>
+      <c r="R77" s="39"/>
+      <c r="S77" s="40"/>
+    </row>
+    <row r="78" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B78" s="41"/>
+      <c r="C78" s="42"/>
+      <c r="D78" s="41"/>
+      <c r="E78" s="43"/>
+      <c r="F78" s="11">
+        <v>0</v>
+      </c>
+      <c r="G78" s="6"/>
+      <c r="H78" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="I77" s="32"/>
-      <c r="J77" s="32"/>
-      <c r="K77" s="32"/>
-      <c r="L77" s="32"/>
-      <c r="M77" s="32"/>
-      <c r="N77" s="32"/>
-      <c r="O77" s="32"/>
-      <c r="P77" s="51"/>
-      <c r="Q77" s="52"/>
-      <c r="R77" s="52"/>
-      <c r="S77" s="53"/>
-    </row>
-    <row r="78" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B78" s="56" t="s">
+      <c r="I78" s="28"/>
+      <c r="J78" s="28"/>
+      <c r="K78" s="28"/>
+      <c r="L78" s="28"/>
+      <c r="M78" s="28"/>
+      <c r="N78" s="28"/>
+      <c r="O78" s="28"/>
+      <c r="P78" s="45"/>
+      <c r="Q78" s="46"/>
+      <c r="R78" s="46"/>
+      <c r="S78" s="47"/>
+    </row>
+    <row r="79" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B79" s="26" t="s">
         <v>168</v>
       </c>
-      <c r="C78" s="56"/>
-      <c r="D78" s="56" t="s">
+      <c r="C79" s="26"/>
+      <c r="D79" s="26" t="s">
         <v>169</v>
       </c>
-      <c r="E78" s="29"/>
-      <c r="F78" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G78" s="6"/>
-      <c r="H78" s="32" t="s">
-        <v>170</v>
-      </c>
-      <c r="I78" s="32"/>
-      <c r="J78" s="32"/>
-      <c r="K78" s="32"/>
-      <c r="L78" s="32"/>
-      <c r="M78" s="32"/>
-      <c r="N78" s="32"/>
-      <c r="O78" s="32"/>
-      <c r="P78" s="32" t="s">
-        <v>171</v>
-      </c>
-      <c r="Q78" s="32"/>
-      <c r="R78" s="32"/>
-      <c r="S78" s="32"/>
-    </row>
-    <row r="79" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B79" s="56" t="s">
-        <v>172</v>
-      </c>
-      <c r="C79" s="56"/>
-      <c r="D79" s="56" t="s">
-        <v>173</v>
-      </c>
-      <c r="E79" s="29"/>
+      <c r="E79" s="27"/>
       <c r="F79" s="5" t="s">
         <v>8</v>
       </c>
       <c r="G79" s="6"/>
-      <c r="H79" s="32" t="s">
+      <c r="H79" s="28" t="s">
+        <v>170</v>
+      </c>
+      <c r="I79" s="28"/>
+      <c r="J79" s="28"/>
+      <c r="K79" s="28"/>
+      <c r="L79" s="28"/>
+      <c r="M79" s="28"/>
+      <c r="N79" s="28"/>
+      <c r="O79" s="28"/>
+      <c r="P79" s="28" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q79" s="28"/>
+      <c r="R79" s="28"/>
+      <c r="S79" s="28"/>
+    </row>
+    <row r="80" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B80" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="C80" s="26"/>
+      <c r="D80" s="26" t="s">
+        <v>173</v>
+      </c>
+      <c r="E80" s="27"/>
+      <c r="F80" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G80" s="6"/>
+      <c r="H80" s="28" t="s">
         <v>174</v>
       </c>
-      <c r="I79" s="32"/>
-      <c r="J79" s="32"/>
-      <c r="K79" s="32"/>
-      <c r="L79" s="32"/>
-      <c r="M79" s="32"/>
-      <c r="N79" s="32"/>
-      <c r="O79" s="32"/>
-      <c r="P79" s="32" t="s">
+      <c r="I80" s="28"/>
+      <c r="J80" s="28"/>
+      <c r="K80" s="28"/>
+      <c r="L80" s="28"/>
+      <c r="M80" s="28"/>
+      <c r="N80" s="28"/>
+      <c r="O80" s="28"/>
+      <c r="P80" s="28" t="s">
         <v>171</v>
       </c>
-      <c r="Q79" s="32"/>
-      <c r="R79" s="32"/>
-      <c r="S79" s="32"/>
-    </row>
-    <row r="80" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B80" s="36" t="s">
+      <c r="Q80" s="28"/>
+      <c r="R80" s="28"/>
+      <c r="S80" s="28"/>
+    </row>
+    <row r="81" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B81" s="29" t="s">
         <v>175</v>
       </c>
-      <c r="C80" s="37"/>
-      <c r="D80" s="36" t="s">
+      <c r="C81" s="30"/>
+      <c r="D81" s="29" t="s">
         <v>176</v>
       </c>
-      <c r="E80" s="42"/>
-      <c r="F80" s="5" t="s">
+      <c r="E81" s="33"/>
+      <c r="F81" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G80" s="6"/>
-      <c r="H80" s="32" t="s">
+      <c r="G81" s="6"/>
+      <c r="H81" s="28" t="s">
         <v>177</v>
       </c>
-      <c r="I80" s="32"/>
-      <c r="J80" s="32"/>
-      <c r="K80" s="32"/>
-      <c r="L80" s="32"/>
-      <c r="M80" s="32"/>
-      <c r="N80" s="32"/>
-      <c r="O80" s="32"/>
-      <c r="P80" s="59"/>
-      <c r="Q80" s="46"/>
-      <c r="R80" s="46"/>
-      <c r="S80" s="47"/>
-    </row>
-    <row r="81" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B81" s="36" t="s">
+      <c r="I81" s="28"/>
+      <c r="J81" s="28"/>
+      <c r="K81" s="28"/>
+      <c r="L81" s="28"/>
+      <c r="M81" s="28"/>
+      <c r="N81" s="28"/>
+      <c r="O81" s="28"/>
+      <c r="P81" s="35"/>
+      <c r="Q81" s="36"/>
+      <c r="R81" s="36"/>
+      <c r="S81" s="37"/>
+    </row>
+    <row r="82" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B82" s="29" t="s">
         <v>178</v>
       </c>
-      <c r="C81" s="37"/>
-      <c r="D81" s="36" t="s">
+      <c r="C82" s="30"/>
+      <c r="D82" s="29" t="s">
         <v>179</v>
       </c>
-      <c r="E81" s="42"/>
-      <c r="F81" s="12" t="s">
+      <c r="E82" s="33"/>
+      <c r="F82" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="G81" s="13"/>
-      <c r="H81" s="45" t="s">
+      <c r="G82" s="13"/>
+      <c r="H82" s="44" t="s">
         <v>180</v>
       </c>
-      <c r="I81" s="46"/>
-      <c r="J81" s="46"/>
-      <c r="K81" s="46"/>
-      <c r="L81" s="46"/>
-      <c r="M81" s="46"/>
-      <c r="N81" s="46"/>
-      <c r="O81" s="47"/>
-      <c r="P81" s="59" t="s">
+      <c r="I82" s="36"/>
+      <c r="J82" s="36"/>
+      <c r="K82" s="36"/>
+      <c r="L82" s="36"/>
+      <c r="M82" s="36"/>
+      <c r="N82" s="36"/>
+      <c r="O82" s="37"/>
+      <c r="P82" s="35" t="s">
         <v>181</v>
       </c>
-      <c r="Q81" s="60"/>
-      <c r="R81" s="60"/>
-      <c r="S81" s="61"/>
-    </row>
-    <row r="82" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B82" s="40"/>
-      <c r="C82" s="41"/>
-      <c r="D82" s="40"/>
-      <c r="E82" s="44"/>
-      <c r="F82" s="14"/>
-      <c r="G82" s="15"/>
-      <c r="H82" s="51"/>
-      <c r="I82" s="52"/>
-      <c r="J82" s="52"/>
-      <c r="K82" s="52"/>
-      <c r="L82" s="52"/>
-      <c r="M82" s="52"/>
-      <c r="N82" s="52"/>
-      <c r="O82" s="53"/>
-      <c r="P82" s="62"/>
-      <c r="Q82" s="63"/>
-      <c r="R82" s="63"/>
-      <c r="S82" s="64"/>
-    </row>
-    <row r="83" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B83" s="36" t="s">
-        <v>182</v>
-      </c>
-      <c r="C83" s="37"/>
-      <c r="D83" s="36" t="s">
-        <v>183</v>
-      </c>
-      <c r="E83" s="42"/>
-      <c r="F83" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="G83" s="13"/>
-      <c r="H83" s="45" t="s">
-        <v>184</v>
-      </c>
+      <c r="Q82" s="48"/>
+      <c r="R82" s="48"/>
+      <c r="S82" s="49"/>
+    </row>
+    <row r="83" spans="2:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B83" s="41"/>
+      <c r="C83" s="42"/>
+      <c r="D83" s="41"/>
+      <c r="E83" s="43"/>
+      <c r="F83" s="14"/>
+      <c r="G83" s="15"/>
+      <c r="H83" s="45"/>
       <c r="I83" s="46"/>
       <c r="J83" s="46"/>
       <c r="K83" s="46"/>
@@ -4288,415 +4299,247 @@
       <c r="M83" s="46"/>
       <c r="N83" s="46"/>
       <c r="O83" s="47"/>
-      <c r="P83" s="59" t="s">
+      <c r="P83" s="50"/>
+      <c r="Q83" s="51"/>
+      <c r="R83" s="51"/>
+      <c r="S83" s="52"/>
+    </row>
+    <row r="84" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B84" s="29" t="s">
+        <v>182</v>
+      </c>
+      <c r="C84" s="30"/>
+      <c r="D84" s="29" t="s">
+        <v>183</v>
+      </c>
+      <c r="E84" s="33"/>
+      <c r="F84" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="G84" s="13"/>
+      <c r="H84" s="44" t="s">
+        <v>184</v>
+      </c>
+      <c r="I84" s="36"/>
+      <c r="J84" s="36"/>
+      <c r="K84" s="36"/>
+      <c r="L84" s="36"/>
+      <c r="M84" s="36"/>
+      <c r="N84" s="36"/>
+      <c r="O84" s="37"/>
+      <c r="P84" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="Q83" s="46"/>
-      <c r="R83" s="46"/>
-      <c r="S83" s="47"/>
-    </row>
-    <row r="84" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B84" s="40"/>
-      <c r="C84" s="41"/>
-      <c r="D84" s="40"/>
-      <c r="E84" s="44"/>
-      <c r="F84" s="14"/>
-      <c r="G84" s="15"/>
-      <c r="H84" s="51"/>
-      <c r="I84" s="52"/>
-      <c r="J84" s="52"/>
-      <c r="K84" s="52"/>
-      <c r="L84" s="52"/>
-      <c r="M84" s="52"/>
-      <c r="N84" s="52"/>
-      <c r="O84" s="53"/>
-      <c r="P84" s="51"/>
-      <c r="Q84" s="52"/>
-      <c r="R84" s="52"/>
-      <c r="S84" s="53"/>
+      <c r="Q84" s="36"/>
+      <c r="R84" s="36"/>
+      <c r="S84" s="37"/>
     </row>
     <row r="85" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B85" s="36" t="s">
-        <v>185</v>
-      </c>
-      <c r="C85" s="37"/>
-      <c r="D85" s="36" t="s">
-        <v>186</v>
-      </c>
-      <c r="E85" s="42"/>
-      <c r="F85" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="G85" s="6"/>
-      <c r="H85" s="32" t="s">
-        <v>188</v>
-      </c>
-      <c r="I85" s="32"/>
-      <c r="J85" s="32"/>
-      <c r="K85" s="32"/>
-      <c r="L85" s="32"/>
-      <c r="M85" s="32"/>
-      <c r="N85" s="32"/>
-      <c r="O85" s="32"/>
+      <c r="B85" s="41"/>
+      <c r="C85" s="42"/>
+      <c r="D85" s="41"/>
+      <c r="E85" s="43"/>
+      <c r="F85" s="14"/>
+      <c r="G85" s="15"/>
+      <c r="H85" s="45"/>
+      <c r="I85" s="46"/>
+      <c r="J85" s="46"/>
+      <c r="K85" s="46"/>
+      <c r="L85" s="46"/>
+      <c r="M85" s="46"/>
+      <c r="N85" s="46"/>
+      <c r="O85" s="47"/>
       <c r="P85" s="45"/>
       <c r="Q85" s="46"/>
       <c r="R85" s="46"/>
       <c r="S85" s="47"/>
     </row>
     <row r="86" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B86" s="38"/>
-      <c r="C86" s="39"/>
-      <c r="D86" s="38"/>
-      <c r="E86" s="43"/>
+      <c r="B86" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="C86" s="30"/>
+      <c r="D86" s="29" t="s">
+        <v>186</v>
+      </c>
+      <c r="E86" s="33"/>
       <c r="F86" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="G86" s="6"/>
+      <c r="H86" s="28" t="s">
+        <v>188</v>
+      </c>
+      <c r="I86" s="28"/>
+      <c r="J86" s="28"/>
+      <c r="K86" s="28"/>
+      <c r="L86" s="28"/>
+      <c r="M86" s="28"/>
+      <c r="N86" s="28"/>
+      <c r="O86" s="28"/>
+      <c r="P86" s="44"/>
+      <c r="Q86" s="36"/>
+      <c r="R86" s="36"/>
+      <c r="S86" s="37"/>
+    </row>
+    <row r="87" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B87" s="31"/>
+      <c r="C87" s="32"/>
+      <c r="D87" s="31"/>
+      <c r="E87" s="34"/>
+      <c r="F87" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="G86" s="6"/>
-      <c r="H86" s="32" t="s">
+      <c r="G87" s="6"/>
+      <c r="H87" s="28" t="s">
         <v>190</v>
       </c>
-      <c r="I86" s="32"/>
-      <c r="J86" s="32"/>
-      <c r="K86" s="32"/>
-      <c r="L86" s="32"/>
-      <c r="M86" s="32"/>
-      <c r="N86" s="32"/>
-      <c r="O86" s="32"/>
-      <c r="P86" s="48"/>
-      <c r="Q86" s="49"/>
-      <c r="R86" s="49"/>
-      <c r="S86" s="50"/>
-    </row>
-    <row r="87" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B87" s="40"/>
-      <c r="C87" s="41"/>
-      <c r="D87" s="40"/>
-      <c r="E87" s="44"/>
-      <c r="F87" s="11">
-        <v>0</v>
-      </c>
-      <c r="G87" s="6"/>
-      <c r="H87" s="32" t="s">
+      <c r="I87" s="28"/>
+      <c r="J87" s="28"/>
+      <c r="K87" s="28"/>
+      <c r="L87" s="28"/>
+      <c r="M87" s="28"/>
+      <c r="N87" s="28"/>
+      <c r="O87" s="28"/>
+      <c r="P87" s="38"/>
+      <c r="Q87" s="39"/>
+      <c r="R87" s="39"/>
+      <c r="S87" s="40"/>
+    </row>
+    <row r="88" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B88" s="41"/>
+      <c r="C88" s="42"/>
+      <c r="D88" s="41"/>
+      <c r="E88" s="43"/>
+      <c r="F88" s="11">
+        <v>0</v>
+      </c>
+      <c r="G88" s="6"/>
+      <c r="H88" s="28" t="s">
         <v>191</v>
       </c>
-      <c r="I87" s="32"/>
-      <c r="J87" s="32"/>
-      <c r="K87" s="32"/>
-      <c r="L87" s="32"/>
-      <c r="M87" s="32"/>
-      <c r="N87" s="32"/>
-      <c r="O87" s="32"/>
-      <c r="P87" s="51"/>
-      <c r="Q87" s="52"/>
-      <c r="R87" s="52"/>
-      <c r="S87" s="53"/>
-    </row>
-    <row r="88" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B88" s="36" t="s">
-        <v>192</v>
-      </c>
-      <c r="C88" s="37"/>
-      <c r="D88" s="36" t="s">
-        <v>193</v>
-      </c>
-      <c r="E88" s="42"/>
-      <c r="F88" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="G88" s="6"/>
-      <c r="H88" s="32" t="s">
-        <v>195</v>
-      </c>
-      <c r="I88" s="32"/>
-      <c r="J88" s="32"/>
-      <c r="K88" s="32"/>
-      <c r="L88" s="32"/>
-      <c r="M88" s="32"/>
-      <c r="N88" s="32"/>
-      <c r="O88" s="32"/>
-      <c r="P88" s="59" t="s">
-        <v>196</v>
-      </c>
+      <c r="I88" s="28"/>
+      <c r="J88" s="28"/>
+      <c r="K88" s="28"/>
+      <c r="L88" s="28"/>
+      <c r="M88" s="28"/>
+      <c r="N88" s="28"/>
+      <c r="O88" s="28"/>
+      <c r="P88" s="45"/>
       <c r="Q88" s="46"/>
       <c r="R88" s="46"/>
       <c r="S88" s="47"/>
     </row>
     <row r="89" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B89" s="38"/>
-      <c r="C89" s="39"/>
-      <c r="D89" s="38"/>
-      <c r="E89" s="43"/>
+      <c r="B89" s="29" t="s">
+        <v>192</v>
+      </c>
+      <c r="C89" s="30"/>
+      <c r="D89" s="29" t="s">
+        <v>193</v>
+      </c>
+      <c r="E89" s="33"/>
       <c r="F89" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="G89" s="6"/>
+      <c r="H89" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="I89" s="28"/>
+      <c r="J89" s="28"/>
+      <c r="K89" s="28"/>
+      <c r="L89" s="28"/>
+      <c r="M89" s="28"/>
+      <c r="N89" s="28"/>
+      <c r="O89" s="28"/>
+      <c r="P89" s="35" t="s">
+        <v>196</v>
+      </c>
+      <c r="Q89" s="36"/>
+      <c r="R89" s="36"/>
+      <c r="S89" s="37"/>
+    </row>
+    <row r="90" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B90" s="31"/>
+      <c r="C90" s="32"/>
+      <c r="D90" s="31"/>
+      <c r="E90" s="34"/>
+      <c r="F90" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="G89" s="6"/>
-      <c r="H89" s="32" t="s">
+      <c r="G90" s="6"/>
+      <c r="H90" s="28" t="s">
         <v>198</v>
       </c>
-      <c r="I89" s="32"/>
-      <c r="J89" s="32"/>
-      <c r="K89" s="32"/>
-      <c r="L89" s="32"/>
-      <c r="M89" s="32"/>
-      <c r="N89" s="32"/>
-      <c r="O89" s="32"/>
-      <c r="P89" s="48"/>
-      <c r="Q89" s="49"/>
-      <c r="R89" s="49"/>
-      <c r="S89" s="50"/>
-    </row>
-    <row r="90" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B90" s="56" t="s">
+      <c r="I90" s="28"/>
+      <c r="J90" s="28"/>
+      <c r="K90" s="28"/>
+      <c r="L90" s="28"/>
+      <c r="M90" s="28"/>
+      <c r="N90" s="28"/>
+      <c r="O90" s="28"/>
+      <c r="P90" s="38"/>
+      <c r="Q90" s="39"/>
+      <c r="R90" s="39"/>
+      <c r="S90" s="40"/>
+    </row>
+    <row r="91" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B91" s="26" t="s">
         <v>199</v>
       </c>
-      <c r="C90" s="56"/>
-      <c r="D90" s="56" t="s">
+      <c r="C91" s="26"/>
+      <c r="D91" s="26" t="s">
         <v>200</v>
       </c>
-      <c r="E90" s="29"/>
-      <c r="F90" s="5" t="s">
+      <c r="E91" s="27"/>
+      <c r="F91" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="G90" s="6"/>
-      <c r="H90" s="32"/>
-      <c r="I90" s="32"/>
-      <c r="J90" s="32"/>
-      <c r="K90" s="32"/>
-      <c r="L90" s="32"/>
-      <c r="M90" s="32"/>
-      <c r="N90" s="32"/>
-      <c r="O90" s="32"/>
-      <c r="P90" s="32"/>
-      <c r="Q90" s="32"/>
-      <c r="R90" s="32"/>
-      <c r="S90" s="32"/>
-    </row>
-    <row r="91" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B91" s="56" t="s">
+      <c r="G91" s="6"/>
+      <c r="H91" s="28"/>
+      <c r="I91" s="28"/>
+      <c r="J91" s="28"/>
+      <c r="K91" s="28"/>
+      <c r="L91" s="28"/>
+      <c r="M91" s="28"/>
+      <c r="N91" s="28"/>
+      <c r="O91" s="28"/>
+      <c r="P91" s="28"/>
+      <c r="Q91" s="28"/>
+      <c r="R91" s="28"/>
+      <c r="S91" s="28"/>
+    </row>
+    <row r="92" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B92" s="26" t="s">
         <v>202</v>
       </c>
-      <c r="C91" s="56"/>
-      <c r="D91" s="56" t="s">
+      <c r="C92" s="26"/>
+      <c r="D92" s="26" t="s">
         <v>203</v>
       </c>
-      <c r="E91" s="29"/>
-      <c r="F91" s="5" t="s">
+      <c r="E92" s="27"/>
+      <c r="F92" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="G91" s="6"/>
-      <c r="H91" s="32"/>
-      <c r="I91" s="32"/>
-      <c r="J91" s="32"/>
-      <c r="K91" s="32"/>
-      <c r="L91" s="32"/>
-      <c r="M91" s="32"/>
-      <c r="N91" s="32"/>
-      <c r="O91" s="32"/>
-      <c r="P91" s="32" t="s">
+      <c r="G92" s="6"/>
+      <c r="H92" s="28"/>
+      <c r="I92" s="28"/>
+      <c r="J92" s="28"/>
+      <c r="K92" s="28"/>
+      <c r="L92" s="28"/>
+      <c r="M92" s="28"/>
+      <c r="N92" s="28"/>
+      <c r="O92" s="28"/>
+      <c r="P92" s="28" t="s">
         <v>205</v>
       </c>
-      <c r="Q91" s="32"/>
-      <c r="R91" s="32"/>
-      <c r="S91" s="32"/>
+      <c r="Q92" s="28"/>
+      <c r="R92" s="28"/>
+      <c r="S92" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="205">
-    <mergeCell ref="B91:C91"/>
-    <mergeCell ref="D91:E91"/>
-    <mergeCell ref="H91:O91"/>
-    <mergeCell ref="P91:S91"/>
-    <mergeCell ref="B88:C89"/>
-    <mergeCell ref="D88:E89"/>
-    <mergeCell ref="H88:O88"/>
-    <mergeCell ref="P88:S89"/>
-    <mergeCell ref="H89:O89"/>
-    <mergeCell ref="B90:C90"/>
-    <mergeCell ref="D90:E90"/>
-    <mergeCell ref="H90:O90"/>
-    <mergeCell ref="P90:S90"/>
-    <mergeCell ref="B83:C84"/>
-    <mergeCell ref="D83:E84"/>
-    <mergeCell ref="H83:O84"/>
-    <mergeCell ref="P83:S84"/>
-    <mergeCell ref="B85:C87"/>
-    <mergeCell ref="D85:E87"/>
-    <mergeCell ref="H85:O85"/>
-    <mergeCell ref="P85:S87"/>
-    <mergeCell ref="H86:O86"/>
-    <mergeCell ref="H87:O87"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="H80:O80"/>
-    <mergeCell ref="P80:S80"/>
-    <mergeCell ref="B81:C82"/>
-    <mergeCell ref="D81:E82"/>
-    <mergeCell ref="H81:O82"/>
-    <mergeCell ref="P81:S82"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="D78:E78"/>
-    <mergeCell ref="H78:O78"/>
-    <mergeCell ref="P78:S78"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="D79:E79"/>
-    <mergeCell ref="H79:O79"/>
-    <mergeCell ref="P79:S79"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="H74:O74"/>
-    <mergeCell ref="P74:S74"/>
-    <mergeCell ref="B75:C77"/>
-    <mergeCell ref="D75:E77"/>
-    <mergeCell ref="H75:O75"/>
-    <mergeCell ref="P75:S77"/>
-    <mergeCell ref="H76:O76"/>
-    <mergeCell ref="H77:O77"/>
-    <mergeCell ref="B71:C73"/>
-    <mergeCell ref="D71:E73"/>
-    <mergeCell ref="H71:O71"/>
-    <mergeCell ref="P71:S73"/>
-    <mergeCell ref="H72:O72"/>
-    <mergeCell ref="H73:O73"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="F68:G68"/>
-    <mergeCell ref="H68:O68"/>
-    <mergeCell ref="P68:S68"/>
-    <mergeCell ref="B69:C70"/>
-    <mergeCell ref="D69:E70"/>
-    <mergeCell ref="H69:O69"/>
-    <mergeCell ref="P69:S70"/>
-    <mergeCell ref="H70:O70"/>
-    <mergeCell ref="B62:C63"/>
-    <mergeCell ref="D62:E63"/>
-    <mergeCell ref="H62:O62"/>
-    <mergeCell ref="P62:S62"/>
-    <mergeCell ref="H63:O63"/>
-    <mergeCell ref="P63:S63"/>
-    <mergeCell ref="B58:C59"/>
-    <mergeCell ref="D58:E59"/>
-    <mergeCell ref="H58:O59"/>
-    <mergeCell ref="P58:S59"/>
-    <mergeCell ref="B60:C61"/>
-    <mergeCell ref="D60:E61"/>
-    <mergeCell ref="H60:O60"/>
-    <mergeCell ref="P60:S61"/>
-    <mergeCell ref="H61:O61"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="H56:O56"/>
-    <mergeCell ref="P56:S56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="H57:O57"/>
-    <mergeCell ref="P57:S57"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="H54:O54"/>
-    <mergeCell ref="P54:S54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="H55:O55"/>
-    <mergeCell ref="P55:S55"/>
-    <mergeCell ref="B51:C53"/>
-    <mergeCell ref="D51:E53"/>
-    <mergeCell ref="H51:O51"/>
-    <mergeCell ref="P51:S53"/>
-    <mergeCell ref="H52:O52"/>
-    <mergeCell ref="H53:O53"/>
-    <mergeCell ref="B48:C49"/>
-    <mergeCell ref="D48:E49"/>
-    <mergeCell ref="H48:O49"/>
-    <mergeCell ref="P48:S49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="H50:O50"/>
-    <mergeCell ref="P50:S50"/>
-    <mergeCell ref="B38:C47"/>
-    <mergeCell ref="D38:E47"/>
-    <mergeCell ref="H38:O38"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="H32:O32"/>
-    <mergeCell ref="P38:S47"/>
-    <mergeCell ref="H39:O39"/>
-    <mergeCell ref="H40:O40"/>
-    <mergeCell ref="H41:O41"/>
-    <mergeCell ref="H42:O42"/>
-    <mergeCell ref="H43:O43"/>
-    <mergeCell ref="H44:O44"/>
-    <mergeCell ref="H45:O45"/>
-    <mergeCell ref="H46:O46"/>
-    <mergeCell ref="H47:O47"/>
-    <mergeCell ref="P32:S32"/>
-    <mergeCell ref="B33:C37"/>
-    <mergeCell ref="D33:E37"/>
-    <mergeCell ref="H33:O33"/>
-    <mergeCell ref="P33:S37"/>
-    <mergeCell ref="H34:O34"/>
-    <mergeCell ref="H35:O35"/>
-    <mergeCell ref="H36:O36"/>
-    <mergeCell ref="H37:O37"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="H22:O22"/>
-    <mergeCell ref="P22:S22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="H23:O23"/>
-    <mergeCell ref="P23:S23"/>
-    <mergeCell ref="B24:C25"/>
-    <mergeCell ref="D24:E25"/>
-    <mergeCell ref="H24:O25"/>
-    <mergeCell ref="P24:S25"/>
-    <mergeCell ref="B26:C27"/>
-    <mergeCell ref="D26:E27"/>
-    <mergeCell ref="H26:O26"/>
-    <mergeCell ref="P26:S27"/>
-    <mergeCell ref="H27:O27"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="H14:O14"/>
-    <mergeCell ref="P14:S14"/>
-    <mergeCell ref="B15:C17"/>
-    <mergeCell ref="D15:E17"/>
-    <mergeCell ref="H15:O15"/>
-    <mergeCell ref="P15:S17"/>
-    <mergeCell ref="H16:O16"/>
-    <mergeCell ref="H17:O17"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="H12:O12"/>
-    <mergeCell ref="P12:S12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="H13:O13"/>
-    <mergeCell ref="P13:S13"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="H10:O10"/>
-    <mergeCell ref="P10:S10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="H11:O11"/>
-    <mergeCell ref="P11:S11"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="H8:O8"/>
-    <mergeCell ref="P8:S8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="H9:O9"/>
-    <mergeCell ref="P9:S9"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="H6:O6"/>
-    <mergeCell ref="P6:S6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="H7:O7"/>
-    <mergeCell ref="P7:S7"/>
+  <mergeCells count="209">
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="F4:G4"/>
@@ -4706,6 +4549,206 @@
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="H5:O5"/>
     <mergeCell ref="P5:S5"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="H9:O9"/>
+    <mergeCell ref="P9:S9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="H10:O10"/>
+    <mergeCell ref="P10:S10"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="H6:O6"/>
+    <mergeCell ref="P6:S6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="H7:O7"/>
+    <mergeCell ref="P7:S7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="H8:O8"/>
+    <mergeCell ref="P8:S8"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="H13:O13"/>
+    <mergeCell ref="P13:S13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="H14:O14"/>
+    <mergeCell ref="P14:S14"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="H11:O11"/>
+    <mergeCell ref="P11:S11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="H12:O12"/>
+    <mergeCell ref="P12:S12"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="H15:O15"/>
+    <mergeCell ref="P15:S15"/>
+    <mergeCell ref="B16:C18"/>
+    <mergeCell ref="D16:E18"/>
+    <mergeCell ref="H16:O16"/>
+    <mergeCell ref="P16:S18"/>
+    <mergeCell ref="H17:O17"/>
+    <mergeCell ref="H18:O18"/>
+    <mergeCell ref="H37:O37"/>
+    <mergeCell ref="H38:O38"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="H23:O23"/>
+    <mergeCell ref="P23:S23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="H24:O24"/>
+    <mergeCell ref="P24:S24"/>
+    <mergeCell ref="B25:C26"/>
+    <mergeCell ref="D25:E26"/>
+    <mergeCell ref="H25:O26"/>
+    <mergeCell ref="P25:S26"/>
+    <mergeCell ref="B27:C28"/>
+    <mergeCell ref="D27:E28"/>
+    <mergeCell ref="H27:O27"/>
+    <mergeCell ref="P27:S28"/>
+    <mergeCell ref="H28:O28"/>
+    <mergeCell ref="B39:C48"/>
+    <mergeCell ref="D39:E48"/>
+    <mergeCell ref="H39:O39"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="H33:O33"/>
+    <mergeCell ref="P39:S48"/>
+    <mergeCell ref="H40:O40"/>
+    <mergeCell ref="H41:O41"/>
+    <mergeCell ref="H42:O42"/>
+    <mergeCell ref="H43:O43"/>
+    <mergeCell ref="H44:O44"/>
+    <mergeCell ref="H45:O45"/>
+    <mergeCell ref="H46:O46"/>
+    <mergeCell ref="H47:O47"/>
+    <mergeCell ref="H48:O48"/>
+    <mergeCell ref="P33:S33"/>
+    <mergeCell ref="B34:C38"/>
+    <mergeCell ref="D34:E38"/>
+    <mergeCell ref="H34:O34"/>
+    <mergeCell ref="P34:S38"/>
+    <mergeCell ref="H35:O35"/>
+    <mergeCell ref="H36:O36"/>
+    <mergeCell ref="B52:C54"/>
+    <mergeCell ref="D52:E54"/>
+    <mergeCell ref="H52:O52"/>
+    <mergeCell ref="P52:S54"/>
+    <mergeCell ref="H53:O53"/>
+    <mergeCell ref="H54:O54"/>
+    <mergeCell ref="B49:C50"/>
+    <mergeCell ref="D49:E50"/>
+    <mergeCell ref="H49:O50"/>
+    <mergeCell ref="P49:S50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="H51:O51"/>
+    <mergeCell ref="P51:S51"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="H57:O57"/>
+    <mergeCell ref="P57:S57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="H58:O58"/>
+    <mergeCell ref="P58:S58"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="H55:O55"/>
+    <mergeCell ref="P55:S55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="H56:O56"/>
+    <mergeCell ref="P56:S56"/>
+    <mergeCell ref="B63:C64"/>
+    <mergeCell ref="D63:E64"/>
+    <mergeCell ref="H63:O63"/>
+    <mergeCell ref="P63:S63"/>
+    <mergeCell ref="H64:O64"/>
+    <mergeCell ref="P64:S64"/>
+    <mergeCell ref="B59:C60"/>
+    <mergeCell ref="D59:E60"/>
+    <mergeCell ref="H59:O60"/>
+    <mergeCell ref="P59:S60"/>
+    <mergeCell ref="B61:C62"/>
+    <mergeCell ref="D61:E62"/>
+    <mergeCell ref="H61:O61"/>
+    <mergeCell ref="P61:S62"/>
+    <mergeCell ref="H62:O62"/>
+    <mergeCell ref="B72:C74"/>
+    <mergeCell ref="D72:E74"/>
+    <mergeCell ref="H72:O72"/>
+    <mergeCell ref="P72:S74"/>
+    <mergeCell ref="H73:O73"/>
+    <mergeCell ref="H74:O74"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="F69:G69"/>
+    <mergeCell ref="H69:O69"/>
+    <mergeCell ref="P69:S69"/>
+    <mergeCell ref="B70:C71"/>
+    <mergeCell ref="D70:E71"/>
+    <mergeCell ref="H70:O70"/>
+    <mergeCell ref="P70:S71"/>
+    <mergeCell ref="H71:O71"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="H75:O75"/>
+    <mergeCell ref="P75:S75"/>
+    <mergeCell ref="B76:C78"/>
+    <mergeCell ref="D76:E78"/>
+    <mergeCell ref="H76:O76"/>
+    <mergeCell ref="P76:S78"/>
+    <mergeCell ref="H77:O77"/>
+    <mergeCell ref="H78:O78"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="H81:O81"/>
+    <mergeCell ref="P81:S81"/>
+    <mergeCell ref="B82:C83"/>
+    <mergeCell ref="D82:E83"/>
+    <mergeCell ref="H82:O83"/>
+    <mergeCell ref="P82:S83"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="D79:E79"/>
+    <mergeCell ref="H79:O79"/>
+    <mergeCell ref="P79:S79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="H80:O80"/>
+    <mergeCell ref="P80:S80"/>
+    <mergeCell ref="B84:C85"/>
+    <mergeCell ref="D84:E85"/>
+    <mergeCell ref="H84:O85"/>
+    <mergeCell ref="P84:S85"/>
+    <mergeCell ref="B86:C88"/>
+    <mergeCell ref="D86:E88"/>
+    <mergeCell ref="H86:O86"/>
+    <mergeCell ref="P86:S88"/>
+    <mergeCell ref="H87:O87"/>
+    <mergeCell ref="H88:O88"/>
+    <mergeCell ref="B92:C92"/>
+    <mergeCell ref="D92:E92"/>
+    <mergeCell ref="H92:O92"/>
+    <mergeCell ref="P92:S92"/>
+    <mergeCell ref="B89:C90"/>
+    <mergeCell ref="D89:E90"/>
+    <mergeCell ref="H89:O89"/>
+    <mergeCell ref="P89:S90"/>
+    <mergeCell ref="H90:O90"/>
+    <mergeCell ref="B91:C91"/>
+    <mergeCell ref="D91:E91"/>
+    <mergeCell ref="H91:O91"/>
+    <mergeCell ref="P91:S91"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4718,7 +4761,7 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -6959,8 +7002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E800857-8593-4BC1-8E06-11FBEDB3FF54}">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>